<commit_message>
updated parameters for eval_by_state
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BioLocE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8718D2-74B2-B445-B6CE-FB476D3DCEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD320B5C-022E-1B45-A351-6E79BD81E0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -620,7 +620,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B45" sqref="B45"/>
+      <selection pane="topRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix issues with evaluation
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\BLocS\blocs\incentives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD320B5C-022E-1B45-A351-6E79BD81E0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E4A58-22B7-4050-8943-E47F027DC841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>State</t>
   </si>
@@ -197,24 +197,6 @@
   </si>
   <si>
     <t>Location Capital Cost Factor (dimensionless)</t>
-  </si>
-  <si>
-    <t>Incentives Available</t>
-  </si>
-  <si>
-    <t>8,9</t>
-  </si>
-  <si>
-    <t>1,12,21</t>
-  </si>
-  <si>
-    <t>13,14,22</t>
-  </si>
-  <si>
-    <t>4,23</t>
-  </si>
-  <si>
-    <t>16,17</t>
   </si>
   <si>
     <t>State Motor Fuel Tax (decimal)</t>
@@ -616,16 +598,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0865C41F-F8C1-F743-9CC7-E8990FCDD1B0}">
-  <dimension ref="A1:P119"/>
+  <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P12" sqref="P12"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,10 +624,10 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>52</v>
@@ -648,28 +636,25 @@
         <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -691,23 +676,20 @@
       <c r="G2" s="4">
         <v>0.82354978354978503</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="H2" s="6">
         <v>0.46</v>
       </c>
+      <c r="I2" s="4">
+        <v>0.48249069999999999</v>
+      </c>
       <c r="J2" s="4">
-        <v>0.48249069999999999</v>
+        <v>0.14291338582677166</v>
       </c>
       <c r="K2" s="4">
-        <v>0.14291338582677166</v>
-      </c>
-      <c r="L2" s="4">
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -729,19 +711,19 @@
       <c r="G3" s="4">
         <v>2.5634722222222202</v>
       </c>
-      <c r="I3">
+      <c r="H3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="J3" s="4">
+      <c r="I3" s="4">
         <v>0.50515179999999993</v>
       </c>
+      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -763,23 +745,23 @@
       <c r="G4" s="4">
         <v>0.95596153846153598</v>
       </c>
-      <c r="I4">
+      <c r="H4">
         <v>0.36</v>
       </c>
+      <c r="I4" s="4">
+        <v>0.65622580000000008</v>
+      </c>
       <c r="J4" s="4">
-        <v>0.65622580000000008</v>
+        <v>0.18622047244094492</v>
       </c>
       <c r="K4" s="4">
-        <v>0.18622047244094492</v>
-      </c>
-      <c r="L4" s="4">
         <v>9.8651913243245778E-2</v>
       </c>
+      <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -801,23 +783,23 @@
       <c r="G5" s="4">
         <v>0.85480952380952302</v>
       </c>
-      <c r="I5">
+      <c r="H5">
         <v>0.66</v>
       </c>
+      <c r="I5" s="4">
+        <v>0.48249069999999999</v>
+      </c>
       <c r="J5" s="4">
-        <v>0.48249069999999999</v>
+        <v>0.14527559055118111</v>
       </c>
       <c r="K5" s="4">
-        <v>0.14527559055118111</v>
-      </c>
-      <c r="L5" s="4">
         <v>0.1</v>
       </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -839,23 +821,23 @@
       <c r="G6" s="4">
         <v>1.0981586402266199</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>0.22</v>
       </c>
+      <c r="I6" s="4">
+        <v>0.61090359999999999</v>
+      </c>
       <c r="J6" s="4">
-        <v>0.61090359999999999</v>
+        <v>0.1846456692913386</v>
       </c>
       <c r="K6" s="4">
-        <v>0.1846456692913386</v>
-      </c>
-      <c r="L6" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
+      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -878,25 +860,22 @@
         <v>0.99910614525139696</v>
       </c>
       <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
         <v>0.36</v>
       </c>
+      <c r="I7" s="4">
+        <v>0.63356469999999998</v>
+      </c>
       <c r="J7" s="4">
-        <v>0.63356469999999998</v>
+        <v>0.13464566929133859</v>
       </c>
       <c r="K7" s="4">
-        <v>0.13464566929133859</v>
-      </c>
-      <c r="L7" s="4">
         <v>0.10100000000000001</v>
       </c>
+      <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -918,19 +897,19 @@
       <c r="G8" s="4">
         <v>1.11506849315068</v>
       </c>
-      <c r="I8">
+      <c r="H8">
         <v>0.26</v>
       </c>
-      <c r="J8" s="4">
+      <c r="I8" s="4">
         <v>0.4673833</v>
       </c>
+      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -952,23 +931,23 @@
       <c r="G9" s="4">
         <v>1.04588235294117</v>
       </c>
-      <c r="I9">
+      <c r="H9">
         <v>0.47</v>
       </c>
+      <c r="I9" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J9" s="4">
-        <v>0.4673833</v>
+        <v>0.1610236220472441</v>
       </c>
       <c r="K9" s="4">
-        <v>0.1610236220472441</v>
-      </c>
-      <c r="L9" s="4">
         <v>0.107</v>
       </c>
+      <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -990,26 +969,26 @@
       <c r="G10" s="4">
         <v>0.82572104018912895</v>
       </c>
+      <c r="H10" s="4">
+        <v>0.5</v>
+      </c>
       <c r="I10" s="4">
-        <v>0.5</v>
+        <v>0.474937</v>
       </c>
       <c r="J10" s="4">
-        <v>0.474937</v>
+        <v>0.15472440944881891</v>
       </c>
       <c r="K10" s="4">
-        <v>0.15472440944881891</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="L10" s="4">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="M10" s="4">
         <v>4.0454826894677567E-2</v>
       </c>
+      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1031,23 +1010,23 @@
       <c r="G11" s="4">
         <v>0.90413502109704202</v>
       </c>
-      <c r="I11">
+      <c r="H11">
         <v>0.46</v>
       </c>
+      <c r="I11" s="4">
+        <v>0.474937</v>
+      </c>
       <c r="J11" s="4">
-        <v>0.474937</v>
+        <v>0.15275590551181104</v>
       </c>
       <c r="K11" s="4">
-        <v>0.15275590551181104</v>
-      </c>
-      <c r="L11" s="4">
         <v>0.1</v>
       </c>
+      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1069,25 +1048,22 @@
       <c r="G12" s="4">
         <v>2.4517088607594899</v>
       </c>
-      <c r="H12">
-        <v>11</v>
+      <c r="H12" s="4">
+        <v>0.9</v>
       </c>
       <c r="I12" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="J12" s="4">
         <v>0.50515179999999993</v>
       </c>
+      <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4">
+      <c r="L12" s="4">
         <v>4.4864072332789565E-2</v>
       </c>
+      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1109,23 +1085,23 @@
       <c r="G13" s="4">
         <v>1.0685826771653499</v>
       </c>
-      <c r="I13">
+      <c r="H13">
         <v>0.36</v>
       </c>
+      <c r="I13" s="4">
+        <v>0.55802770000000002</v>
+      </c>
       <c r="J13" s="4">
-        <v>0.55802770000000002</v>
+        <v>0.17480314960629922</v>
       </c>
       <c r="K13" s="4">
-        <v>0.17480314960629922</v>
-      </c>
-      <c r="L13" s="4">
         <v>0.10087370618133218</v>
       </c>
+      <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1147,23 +1123,23 @@
       <c r="G14" s="4">
         <v>1</v>
       </c>
-      <c r="I14">
+      <c r="H14">
         <v>0.66</v>
       </c>
+      <c r="I14" s="4">
+        <v>0.55802770000000002</v>
+      </c>
       <c r="J14" s="4">
-        <v>0.55802770000000002</v>
+        <v>0.13503937007874017</v>
       </c>
       <c r="K14" s="4">
-        <v>0.13503937007874017</v>
-      </c>
-      <c r="L14" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
+      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1185,23 +1161,23 @@
       <c r="G15" s="4">
         <v>0.921747311827955</v>
       </c>
-      <c r="I15">
+      <c r="H15">
         <v>0.66</v>
       </c>
+      <c r="I15" s="4">
+        <v>0.57313510000000001</v>
+      </c>
       <c r="J15" s="4">
-        <v>0.57313510000000001</v>
+        <v>0.14291338582677166</v>
       </c>
       <c r="K15" s="4">
-        <v>0.14291338582677166</v>
-      </c>
-      <c r="L15" s="4">
         <v>0.1</v>
       </c>
+      <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1223,26 +1199,23 @@
       <c r="G16" s="4">
         <v>1.05122881355932</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="6">
+      <c r="H16" s="6">
         <v>0.66</v>
       </c>
+      <c r="I16" s="4">
+        <v>0.56558140000000001</v>
+      </c>
       <c r="J16" s="4">
-        <v>0.56558140000000001</v>
+        <v>0.12992125984251968</v>
       </c>
       <c r="K16" s="4">
-        <v>0.12992125984251968</v>
-      </c>
-      <c r="L16" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
+      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1265,25 +1238,22 @@
         <v>1.02352459016393</v>
       </c>
       <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
         <v>0.55000000000000004</v>
       </c>
+      <c r="I17" s="4">
+        <v>0.67133320000000007</v>
+      </c>
       <c r="J17" s="4">
-        <v>0.67133320000000007</v>
+        <v>0.12598425196850396</v>
       </c>
       <c r="K17" s="4">
-        <v>0.12598425196850396</v>
-      </c>
-      <c r="L17" s="4">
         <v>9.2999999999999999E-2</v>
       </c>
+      <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1305,26 +1275,23 @@
       <c r="G18" s="4">
         <v>0.874117647058822</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="7">
+      <c r="H18" s="7">
         <v>0.46499999999999997</v>
       </c>
+      <c r="I18" s="4">
+        <v>0.49004439999999999</v>
+      </c>
       <c r="J18" s="4">
-        <v>0.49004439999999999</v>
+        <v>0.14724409448818898</v>
       </c>
       <c r="K18" s="4">
-        <v>0.14724409448818898</v>
-      </c>
-      <c r="L18" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
+      <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1346,29 +1313,26 @@
       <c r="G19" s="4">
         <v>0.847694805194804</v>
       </c>
-      <c r="H19">
-        <v>15</v>
+      <c r="H19" s="4">
+        <v>0.55666666666666675</v>
       </c>
       <c r="I19" s="4">
-        <v>0.55666666666666675</v>
+        <v>0.474937</v>
       </c>
       <c r="J19" s="4">
-        <v>0.474937</v>
+        <v>0.1456692913385827</v>
       </c>
       <c r="K19" s="4">
-        <v>0.1456692913385827</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="L19" s="4">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="M19" s="4">
         <v>4.6407308236128764E-2</v>
       </c>
+      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1390,19 +1354,19 @@
       <c r="G20" s="4">
         <v>1.0423026315789401</v>
       </c>
-      <c r="I20">
+      <c r="H20">
         <v>0.26</v>
       </c>
-      <c r="J20" s="4">
+      <c r="I20" s="4">
         <v>0.4673833</v>
       </c>
+      <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1424,23 +1388,23 @@
       <c r="G21" s="4">
         <v>0.98325966850828705</v>
       </c>
-      <c r="I21">
+      <c r="H21">
         <v>0.47</v>
       </c>
+      <c r="I21" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J21" s="4">
-        <v>0.4673833</v>
+        <v>0.15944881889763779</v>
       </c>
       <c r="K21" s="4">
-        <v>0.15944881889763779</v>
-      </c>
-      <c r="L21" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
+      <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1462,19 +1426,19 @@
       <c r="G22" s="4">
         <v>1.17718954248365</v>
       </c>
-      <c r="I22">
+      <c r="H22">
         <v>0.26</v>
       </c>
-      <c r="J22" s="4">
+      <c r="I22" s="4">
         <v>0.474937</v>
       </c>
+      <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1497,25 +1461,22 @@
         <v>1.03088372093023</v>
       </c>
       <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23">
         <v>0.66</v>
       </c>
+      <c r="I23" s="4">
+        <v>0.50515179999999993</v>
+      </c>
       <c r="J23" s="4">
-        <v>0.50515179999999993</v>
+        <v>0.13543307086614173</v>
       </c>
       <c r="K23" s="4">
-        <v>0.13543307086614173</v>
-      </c>
-      <c r="L23" s="4">
         <v>0.10299999999999999</v>
       </c>
+      <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1537,23 +1498,23 @@
       <c r="G24" s="4">
         <v>1.0664848484848399</v>
       </c>
-      <c r="I24">
+      <c r="H24">
         <v>0.66</v>
       </c>
+      <c r="I24" s="4">
+        <v>0.52781290000000003</v>
+      </c>
       <c r="J24" s="4">
-        <v>0.52781290000000003</v>
+        <v>0.12637795275590552</v>
       </c>
       <c r="K24" s="4">
-        <v>0.12637795275590552</v>
-      </c>
-      <c r="L24" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
+      <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1575,23 +1536,23 @@
       <c r="G25" s="4">
         <v>0.91778925619834395</v>
       </c>
-      <c r="I25">
+      <c r="H25">
         <v>0.46</v>
       </c>
+      <c r="I25" s="4">
+        <v>0.53536660000000003</v>
+      </c>
       <c r="J25" s="4">
-        <v>0.53536660000000003</v>
+        <v>0.14724409448818898</v>
       </c>
       <c r="K25" s="4">
-        <v>0.14724409448818898</v>
-      </c>
-      <c r="L25" s="4">
         <v>9.6000000000000002E-2</v>
       </c>
+      <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1613,23 +1574,23 @@
       <c r="G26" s="4">
         <v>1.01294685990338</v>
       </c>
+      <c r="H26" s="4">
+        <v>0.55666666666666675</v>
+      </c>
       <c r="I26" s="4">
-        <v>0.55666666666666675</v>
+        <v>0.57313510000000001</v>
       </c>
       <c r="J26" s="4">
-        <v>0.57313510000000001</v>
+        <v>0.13385826771653545</v>
       </c>
       <c r="K26" s="4">
-        <v>0.13385826771653545</v>
-      </c>
-      <c r="L26" s="4">
         <v>9.0999999999999998E-2</v>
       </c>
+      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1651,23 +1612,20 @@
       <c r="G27" s="4">
         <v>1.12787581699346</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="H27" s="6">
         <v>0.36</v>
       </c>
+      <c r="I27" s="4">
+        <v>0.56558140000000001</v>
+      </c>
       <c r="J27" s="4">
-        <v>0.56558140000000001</v>
+        <v>0.16338582677165356</v>
       </c>
       <c r="K27" s="4">
-        <v>0.16338582677165356</v>
-      </c>
-      <c r="L27" s="4">
         <v>0.10154192194819864</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1689,23 +1647,20 @@
       <c r="G28" s="4">
         <v>0.93129411764706205</v>
       </c>
-      <c r="H28">
-        <v>5</v>
+      <c r="H28" s="4">
+        <v>0.60499999999999998</v>
       </c>
       <c r="I28" s="4">
-        <v>0.60499999999999998</v>
+        <v>0.61090359999999999</v>
       </c>
       <c r="J28" s="4">
-        <v>0.61090359999999999</v>
+        <v>0.13070866141732285</v>
       </c>
       <c r="K28" s="4">
-        <v>0.13070866141732285</v>
-      </c>
-      <c r="L28" s="4">
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1727,16 +1682,16 @@
       <c r="G29" s="4">
         <v>1.2103846153846101</v>
       </c>
-      <c r="I29">
+      <c r="H29">
         <v>0.36</v>
       </c>
-      <c r="J29" s="4">
+      <c r="I29" s="4">
         <v>0.54292030000000002</v>
       </c>
+      <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1758,16 +1713,16 @@
       <c r="G30" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="I30">
+      <c r="H30">
         <v>0.26</v>
       </c>
-      <c r="J30" s="4">
+      <c r="I30" s="4">
         <v>0.4673833</v>
       </c>
+      <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1789,20 +1744,20 @@
       <c r="G31" s="4">
         <v>1.21164062499999</v>
       </c>
-      <c r="I31">
+      <c r="H31">
         <v>0.47</v>
       </c>
+      <c r="I31" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J31" s="4">
-        <v>0.4673833</v>
+        <v>0.15354330708661418</v>
       </c>
       <c r="K31" s="4">
-        <v>0.15354330708661418</v>
-      </c>
-      <c r="L31" s="4">
         <v>0.108</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1825,22 +1780,19 @@
         <v>0.97622641509433805</v>
       </c>
       <c r="H32">
-        <v>7</v>
-      </c>
-      <c r="I32">
         <v>0.36</v>
       </c>
+      <c r="I32" s="4">
+        <v>0.64867209999999997</v>
+      </c>
       <c r="J32" s="4">
-        <v>0.64867209999999997</v>
+        <v>0.15472440944881891</v>
       </c>
       <c r="K32" s="4">
-        <v>0.15472440944881891</v>
-      </c>
-      <c r="L32" s="4">
         <v>0.10101251037412776</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1862,20 +1814,20 @@
       <c r="G33" s="4">
         <v>1.1382673267326699</v>
       </c>
-      <c r="I33">
+      <c r="H33">
         <v>0.26</v>
       </c>
+      <c r="I33" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J33" s="4">
-        <v>0.4673833</v>
+        <v>0.15354330708661418</v>
       </c>
       <c r="K33" s="4">
-        <v>0.15354330708661418</v>
-      </c>
-      <c r="L33" s="4">
         <v>0.104</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1897,20 +1849,20 @@
       <c r="G34" s="4">
         <v>0.884571428571434</v>
       </c>
-      <c r="I34">
+      <c r="H34">
         <v>0.46</v>
       </c>
+      <c r="I34" s="4">
+        <v>0.474937</v>
+      </c>
       <c r="J34" s="4">
-        <v>0.474937</v>
+        <v>0.16023622047244096</v>
       </c>
       <c r="K34" s="4">
-        <v>0.16023622047244096</v>
-      </c>
-      <c r="L34" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1932,20 +1884,20 @@
       <c r="G35" s="4">
         <v>1.06910869565217</v>
       </c>
+      <c r="H35" s="4">
+        <v>0.60499999999999998</v>
+      </c>
       <c r="I35" s="4">
-        <v>0.60499999999999998</v>
+        <v>0.56558140000000001</v>
       </c>
       <c r="J35" s="4">
-        <v>0.56558140000000001</v>
+        <v>0.11850393700787401</v>
       </c>
       <c r="K35" s="4">
-        <v>0.11850393700787401</v>
-      </c>
-      <c r="L35" s="4">
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1967,20 +1919,20 @@
       <c r="G36" s="4">
         <v>0.93595617529880604</v>
       </c>
-      <c r="I36">
+      <c r="H36">
         <v>0.47</v>
       </c>
+      <c r="I36" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J36" s="4">
-        <v>0.4673833</v>
+        <v>0.14212598425196851</v>
       </c>
       <c r="K36" s="4">
-        <v>0.14212598425196851</v>
-      </c>
-      <c r="L36" s="4">
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2002,20 +1954,20 @@
       <c r="G37" s="4">
         <v>0.87760000000000005</v>
       </c>
-      <c r="I37">
+      <c r="H37">
         <v>0.55000000000000004</v>
       </c>
+      <c r="I37" s="4">
+        <v>0.5882425</v>
+      </c>
       <c r="J37" s="4">
-        <v>0.5882425</v>
+        <v>0.13346456692913386</v>
       </c>
       <c r="K37" s="4">
-        <v>0.13346456692913386</v>
-      </c>
-      <c r="L37" s="4">
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2038,22 +1990,19 @@
         <v>1.1080630630630599</v>
       </c>
       <c r="H38">
-        <v>6</v>
-      </c>
-      <c r="I38">
         <v>0.36</v>
       </c>
+      <c r="I38" s="4">
+        <v>0.54292030000000002</v>
+      </c>
       <c r="J38" s="4">
-        <v>0.54292030000000002</v>
+        <v>0.1673228346456693</v>
       </c>
       <c r="K38" s="4">
-        <v>0.1673228346456693</v>
-      </c>
-      <c r="L38" s="4">
         <v>0.10148699597777602</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2075,20 +2024,20 @@
       <c r="G39" s="4">
         <v>1.07753164556962</v>
       </c>
-      <c r="I39">
+      <c r="H39">
         <v>0.47</v>
       </c>
+      <c r="I39" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J39" s="4">
-        <v>0.4673833</v>
+        <v>0.15905511811023623</v>
       </c>
       <c r="K39" s="4">
-        <v>0.15905511811023623</v>
-      </c>
-      <c r="L39" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2110,16 +2059,16 @@
       <c r="G40" s="4">
         <v>1.12333333333333</v>
       </c>
-      <c r="I40">
+      <c r="H40">
         <v>0.26</v>
       </c>
-      <c r="J40" s="4">
+      <c r="I40" s="4">
         <v>0.4673833</v>
       </c>
+      <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2141,23 +2090,20 @@
       <c r="G41" s="4">
         <v>0.93315508021390203</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I41" s="6">
+      <c r="H41" s="6">
         <v>0.46</v>
       </c>
+      <c r="I41" s="4">
+        <v>0.474937</v>
+      </c>
       <c r="J41" s="4">
-        <v>0.474937</v>
+        <v>0.14527559055118111</v>
       </c>
       <c r="K41" s="4">
-        <v>0.14527559055118111</v>
-      </c>
-      <c r="L41" s="4">
         <v>0.104</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2179,20 +2125,20 @@
       <c r="G42" s="4">
         <v>0.99818750000000001</v>
       </c>
+      <c r="H42" s="4">
+        <v>0.60499999999999998</v>
+      </c>
       <c r="I42" s="4">
-        <v>0.60499999999999998</v>
+        <v>0.55047400000000002</v>
       </c>
       <c r="J42" s="4">
-        <v>0.55047400000000002</v>
+        <v>0.12165354330708661</v>
       </c>
       <c r="K42" s="4">
-        <v>0.12165354330708661</v>
-      </c>
-      <c r="L42" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2214,20 +2160,20 @@
       <c r="G43" s="4">
         <v>0.85303763440860003</v>
       </c>
-      <c r="I43">
+      <c r="H43">
         <v>0.46</v>
       </c>
+      <c r="I43" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J43" s="4">
-        <v>0.4673833</v>
+        <v>0.14409448818897638</v>
       </c>
       <c r="K43" s="4">
-        <v>0.14409448818897638</v>
-      </c>
-      <c r="L43" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2249,23 +2195,23 @@
       <c r="G44" s="4">
         <v>0.90491631799163097</v>
       </c>
-      <c r="I44">
+      <c r="H44">
         <v>0.47</v>
       </c>
+      <c r="I44" s="4">
+        <v>0.52781290000000003</v>
+      </c>
       <c r="J44" s="4">
-        <v>0.52781290000000003</v>
+        <v>0.14606299212598425</v>
       </c>
       <c r="K44" s="4">
-        <v>0.14606299212598425</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="L44" s="4">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="M44" s="4">
         <v>2.1495071510795983E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2288,22 +2234,19 @@
         <v>1.07424778761061</v>
       </c>
       <c r="H45">
-        <v>18</v>
-      </c>
-      <c r="I45">
         <v>0.36</v>
       </c>
+      <c r="I45" s="4">
+        <v>0.51270550000000004</v>
+      </c>
       <c r="J45" s="4">
-        <v>0.51270550000000004</v>
+        <v>0.15236220472440945</v>
       </c>
       <c r="K45" s="4">
-        <v>0.15236220472440945</v>
-      </c>
-      <c r="L45" s="4">
         <v>0.10071295241200602</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2325,16 +2268,16 @@
       <c r="G46" s="4">
         <v>1.06</v>
       </c>
-      <c r="I46">
+      <c r="H46">
         <v>0.26</v>
       </c>
-      <c r="J46" s="4">
+      <c r="I46" s="4">
         <v>0.4673833</v>
       </c>
+      <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2357,22 +2300,19 @@
         <v>0.97886292834890798</v>
       </c>
       <c r="H47">
-        <v>19</v>
-      </c>
-      <c r="I47">
         <v>0.47</v>
       </c>
+      <c r="I47" s="4">
+        <v>0.48249069999999999</v>
+      </c>
       <c r="J47" s="4">
-        <v>0.48249069999999999</v>
+        <v>0.15748031496062992</v>
       </c>
       <c r="K47" s="4">
-        <v>0.15748031496062992</v>
-      </c>
-      <c r="L47" s="4">
         <v>0.10100000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2394,20 +2334,20 @@
       <c r="G48" s="4">
         <v>1.1595070422535101</v>
       </c>
-      <c r="I48">
+      <c r="H48">
         <v>0.36</v>
       </c>
+      <c r="I48" s="4">
+        <v>0.56558140000000001</v>
+      </c>
       <c r="J48" s="4">
-        <v>0.56558140000000001</v>
+        <v>0.18543307086614175</v>
       </c>
       <c r="K48" s="4">
-        <v>0.18543307086614175</v>
-      </c>
-      <c r="L48" s="4">
         <v>9.8855017374080478E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2429,20 +2369,20 @@
       <c r="G49" s="4">
         <v>1.00439999999999</v>
       </c>
-      <c r="I49">
+      <c r="H49">
         <v>0.47</v>
       </c>
+      <c r="I49" s="4">
+        <v>0.4673833</v>
+      </c>
       <c r="J49" s="4">
-        <v>0.4673833</v>
+        <v>0.15354330708661418</v>
       </c>
       <c r="K49" s="4">
-        <v>0.15354330708661418</v>
-      </c>
-      <c r="L49" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2464,20 +2404,20 @@
       <c r="G50" s="4">
         <v>1.0709574468084999</v>
       </c>
-      <c r="I50">
+      <c r="H50">
         <v>0.66</v>
       </c>
+      <c r="I50" s="4">
+        <v>0.56558140000000001</v>
+      </c>
       <c r="J50" s="4">
-        <v>0.56558140000000001</v>
+        <v>0.12913385826771653</v>
       </c>
       <c r="K50" s="4">
-        <v>0.12913385826771653</v>
-      </c>
-      <c r="L50" s="4">
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2499,186 +2439,186 @@
       <c r="G51" s="4">
         <v>1.0227906976744101</v>
       </c>
-      <c r="I51">
+      <c r="H51">
         <v>0.36</v>
       </c>
+      <c r="I51" s="4">
+        <v>0.48249069999999999</v>
+      </c>
       <c r="J51" s="4">
-        <v>0.48249069999999999</v>
+        <v>0.13346456692913386</v>
       </c>
       <c r="K51" s="4">
-        <v>0.13346456692913386</v>
-      </c>
-      <c r="L51" s="4">
         <v>9.5922391195530504E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F54" s="3"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B80" s="3"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="3"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="3"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="3"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="3"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="3"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="3"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="3"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="3"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="3"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="3"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="3"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="3"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="3"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="3"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="3"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="3"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="3"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="3"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="3"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="3"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="3"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="3"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="3"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="3"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="3"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="3"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="3"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="3"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="3"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="3"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="3"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="3"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:P26">
-    <sortCondition ref="P3:P26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:O26">
+    <sortCondition ref="O3:O26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update costs to year 2020
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\Code\BLocS\blocs\incentives\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E4A58-22B7-4050-8943-E47F027DC841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92C5ACE-DE4F-6E4C-9561-D913F4303C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -228,7 +231,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,13 +253,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -284,6 +300,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,20 +618,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0865C41F-F8C1-F743-9CC7-E8990FCDD1B0}">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +672,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -671,7 +689,7 @@
         <v>0.04</v>
       </c>
       <c r="F2" s="3">
-        <v>6.0100000000000001E-2</v>
+        <v>6.2789131663139625E-2</v>
       </c>
       <c r="G2" s="4">
         <v>0.82354978354978503</v>
@@ -683,13 +701,13 @@
         <v>0.48249069999999999</v>
       </c>
       <c r="J2" s="4">
-        <v>0.14291338582677166</v>
+        <v>0.15181188116355238</v>
       </c>
       <c r="K2" s="4">
-        <v>0.10100000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.1009798606781888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -706,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>0.17100000000000001</v>
+        <v>0.16386843710989343</v>
       </c>
       <c r="G3" s="4">
         <v>2.5634722222222202</v>
@@ -723,7 +741,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -740,7 +758,7 @@
         <v>5.5999999999999994E-2</v>
       </c>
       <c r="F4" s="3">
-        <v>6.5500000000000003E-2</v>
+        <v>6.6443261853096097E-2</v>
       </c>
       <c r="G4" s="4">
         <v>0.95596153846153598</v>
@@ -752,16 +770,14 @@
         <v>0.65622580000000008</v>
       </c>
       <c r="J4" s="4">
-        <v>0.18622047244094492</v>
-      </c>
-      <c r="K4" s="4">
-        <v>9.8651913243245778E-2</v>
-      </c>
+        <v>0.1828893050111752</v>
+      </c>
+      <c r="K4" s="4"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -778,7 +794,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F5" s="3">
-        <v>5.6399999999999999E-2</v>
+        <v>6.1117582891474474E-2</v>
       </c>
       <c r="G5" s="4">
         <v>0.85480952380952302</v>
@@ -789,17 +805,17 @@
       <c r="I5" s="4">
         <v>0.48249069999999999</v>
       </c>
-      <c r="J5" s="4">
-        <v>0.14527559055118111</v>
+      <c r="J5" s="8">
+        <v>0.14752052802935314</v>
       </c>
       <c r="K5" s="4">
-        <v>0.1</v>
+        <v>9.9827239610366672E-2</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -816,7 +832,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="F6" s="3">
-        <v>0.13200000000000001</v>
+        <v>0.12366670610986258</v>
       </c>
       <c r="G6" s="4">
         <v>1.0981586402266199</v>
@@ -828,16 +844,16 @@
         <v>0.61090359999999999</v>
       </c>
       <c r="J6" s="4">
-        <v>0.1846456692913386</v>
+        <v>0.16425594135119409</v>
       </c>
       <c r="K6" s="4">
-        <v>9.9000000000000005E-2</v>
+        <v>9.9100060902702611E-2</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -854,7 +870,7 @@
         <v>2.8999999999999998E-2</v>
       </c>
       <c r="F7" s="3">
-        <v>7.4700000000000003E-2</v>
+        <v>7.5577173790691177E-2</v>
       </c>
       <c r="G7" s="4">
         <v>0.99910614525139696</v>
@@ -866,16 +882,16 @@
         <v>0.63356469999999998</v>
       </c>
       <c r="J7" s="4">
-        <v>0.13464566929133859</v>
+        <v>0.14313759791125041</v>
       </c>
       <c r="K7" s="4">
-        <v>0.10100000000000001</v>
+        <v>0.1005980543403491</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -892,7 +908,7 @@
         <v>6.3500000000000001E-2</v>
       </c>
       <c r="F8" s="3">
-        <v>0.13769999999999999</v>
+        <v>0.13663525910578617</v>
       </c>
       <c r="G8" s="4">
         <v>1.11506849315068</v>
@@ -909,7 +925,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -926,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>7.9500000000000001E-2</v>
+        <v>8.5310311576788742E-2</v>
       </c>
       <c r="G9" s="4">
         <v>1.04588235294117</v>
@@ -938,16 +954,16 @@
         <v>0.4673833</v>
       </c>
       <c r="J9" s="4">
-        <v>0.1610236220472441</v>
+        <v>0.16286177082103859</v>
       </c>
       <c r="K9" s="4">
-        <v>0.107</v>
+        <v>0.10749740378117047</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -964,7 +980,7 @@
         <v>0.06</v>
       </c>
       <c r="F10" s="3">
-        <v>7.6499999999999999E-2</v>
+        <v>8.2180025132533141E-2</v>
       </c>
       <c r="G10" s="4">
         <v>0.82572104018912895</v>
@@ -976,19 +992,19 @@
         <v>0.474937</v>
       </c>
       <c r="J10" s="4">
-        <v>0.15472440944881891</v>
+        <v>0.15863061458229014</v>
       </c>
       <c r="K10" s="4">
-        <v>0.10100000000000001</v>
+        <v>0.10105252773364543</v>
       </c>
       <c r="L10" s="4">
-        <v>4.0454826894677567E-2</v>
+        <v>3.5460462291237851E-2</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1005,7 +1021,7 @@
         <v>0.04</v>
       </c>
       <c r="F11" s="3">
-        <v>0.06</v>
+        <v>6.3423978207905019E-2</v>
       </c>
       <c r="G11" s="4">
         <v>0.90413502109704202</v>
@@ -1017,16 +1033,16 @@
         <v>0.474937</v>
       </c>
       <c r="J11" s="4">
-        <v>0.15275590551181104</v>
+        <v>0.16518991256398702</v>
       </c>
       <c r="K11" s="4">
-        <v>0.1</v>
+        <v>9.9837507844487458E-2</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1043,7 +1059,7 @@
         <v>0.04</v>
       </c>
       <c r="F12" s="3">
-        <v>0.26100000000000001</v>
+        <v>0.26779016263781885</v>
       </c>
       <c r="G12" s="4">
         <v>2.4517088607594899</v>
@@ -1056,14 +1072,14 @@
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4">
-        <v>4.4864072332789565E-2</v>
+      <c r="L12" s="9">
+        <v>4.1837569088880762E-2</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>0.06</v>
       </c>
       <c r="F13" s="3">
-        <v>6.4699999999999994E-2</v>
+        <v>6.2761533922631604E-2</v>
       </c>
       <c r="G13" s="4">
         <v>1.0685826771653499</v>
@@ -1092,16 +1108,14 @@
         <v>0.55802770000000002</v>
       </c>
       <c r="J13" s="4">
-        <v>0.17480314960629922</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0.10087370618133218</v>
-      </c>
+        <v>0.16377798277399688</v>
+      </c>
+      <c r="K13" s="4"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1118,7 +1132,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="F14" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>6.7262441783450463E-2</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
@@ -1130,16 +1144,16 @@
         <v>0.55802770000000002</v>
       </c>
       <c r="J14" s="4">
-        <v>0.13503937007874017</v>
+        <v>0.14211697862500514</v>
       </c>
       <c r="K14" s="4">
-        <v>9.9000000000000005E-2</v>
+        <v>9.9247241347447446E-2</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1156,7 +1170,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F15" s="3">
-        <v>7.3800000000000004E-2</v>
+        <v>7.0590290596535779E-2</v>
       </c>
       <c r="G15" s="4">
         <v>0.921747311827955</v>
@@ -1168,16 +1182,16 @@
         <v>0.57313510000000001</v>
       </c>
       <c r="J15" s="4">
-        <v>0.14291338582677166</v>
+        <v>0.14771147761180747</v>
       </c>
       <c r="K15" s="4">
-        <v>0.1</v>
+        <v>9.9621976671312243E-2</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1194,7 +1208,7 @@
         <v>0.06</v>
       </c>
       <c r="F16" s="3">
-        <v>6.4500000000000002E-2</v>
+        <v>6.0891019236762482E-2</v>
       </c>
       <c r="G16" s="4">
         <v>1.05122881355932</v>
@@ -1206,16 +1220,16 @@
         <v>0.56558140000000001</v>
       </c>
       <c r="J16" s="4">
-        <v>0.12992125984251968</v>
+        <v>0.14093735809892324</v>
       </c>
       <c r="K16" s="4">
-        <v>9.8000000000000004E-2</v>
+        <v>9.7590485058197077E-2</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1232,7 +1246,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F17" s="3">
-        <v>7.5999999999999998E-2</v>
+        <v>7.5327301796108095E-2</v>
       </c>
       <c r="G17" s="4">
         <v>1.02352459016393</v>
@@ -1244,16 +1258,16 @@
         <v>0.67133320000000007</v>
       </c>
       <c r="J17" s="4">
-        <v>0.12598425196850396</v>
+        <v>0.13986471749870394</v>
       </c>
       <c r="K17" s="4">
-        <v>9.2999999999999999E-2</v>
+        <v>9.3021849274127308E-2</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1284,7 @@
         <v>0.06</v>
       </c>
       <c r="F18" s="3">
-        <v>5.6800000000000003E-2</v>
+        <v>5.6937146951795831E-2</v>
       </c>
       <c r="G18" s="4">
         <v>0.874117647058822</v>
@@ -1282,16 +1296,16 @@
         <v>0.49004439999999999</v>
       </c>
       <c r="J18" s="4">
-        <v>0.14724409448818898</v>
+        <v>0.14826754107153112</v>
       </c>
       <c r="K18" s="4">
-        <v>9.5000000000000001E-2</v>
+        <v>9.4899700034390674E-2</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1308,7 +1322,7 @@
         <v>4.4500000000000005E-2</v>
       </c>
       <c r="F19" s="3">
-        <v>5.3499999999999999E-2</v>
+        <v>5.6230227333412305E-2</v>
       </c>
       <c r="G19" s="4">
         <v>0.847694805194804</v>
@@ -1320,19 +1334,19 @@
         <v>0.474937</v>
       </c>
       <c r="J19" s="4">
-        <v>0.1456692913385827</v>
+        <v>0.14599419409541536</v>
       </c>
       <c r="K19" s="4">
-        <v>9.9000000000000005E-2</v>
+        <v>9.904545674243613E-2</v>
       </c>
       <c r="L19" s="4">
-        <v>4.6407308236128764E-2</v>
+        <v>3.0998164400037817E-2</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1349,7 +1363,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="F20" s="3">
-        <v>9.3200000000000005E-2</v>
+        <v>9.215547040094374E-2</v>
       </c>
       <c r="G20" s="4">
         <v>1.0423026315789401</v>
@@ -1366,7 +1380,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>0.06</v>
       </c>
       <c r="F21" s="3">
-        <v>8.2299999999999998E-2</v>
+        <v>8.716104866626935E-2</v>
       </c>
       <c r="G21" s="4">
         <v>0.98325966850828705</v>
@@ -1394,17 +1408,17 @@
       <c r="I21" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J21" s="4">
-        <v>0.15944881889763779</v>
+      <c r="J21" s="8">
+        <v>0.16096259395991458</v>
       </c>
       <c r="K21" s="4">
-        <v>9.8000000000000004E-2</v>
+        <v>9.7668460825379097E-2</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1421,7 +1435,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="F22" s="3">
-        <v>0.1489</v>
+        <v>0.14155008620047138</v>
       </c>
       <c r="G22" s="4">
         <v>1.17718954248365</v>
@@ -1438,7 +1452,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1469,7 @@
         <v>0.06</v>
       </c>
       <c r="F23" s="3">
-        <v>7.0999999999999994E-2</v>
+        <v>7.5334071429621285E-2</v>
       </c>
       <c r="G23" s="4">
         <v>1.03088372093023</v>
@@ -1466,17 +1480,17 @@
       <c r="I23" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="J23" s="4">
-        <v>0.13543307086614173</v>
+      <c r="J23" s="8">
+        <v>0.14361676480793545</v>
       </c>
       <c r="K23" s="4">
-        <v>0.10299999999999999</v>
+        <v>0.10254721620128734</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1493,7 +1507,7 @@
         <v>6.8750000000000006E-2</v>
       </c>
       <c r="F24" s="3">
-        <v>7.5200000000000003E-2</v>
+        <v>7.28318797422043E-2</v>
       </c>
       <c r="G24" s="4">
         <v>1.0664848484848399</v>
@@ -1505,16 +1519,16 @@
         <v>0.52781290000000003</v>
       </c>
       <c r="J24" s="4">
-        <v>0.12637795275590552</v>
+        <v>0.13573154763419962</v>
       </c>
       <c r="K24" s="4">
-        <v>9.6000000000000002E-2</v>
+        <v>9.6428935997652065E-2</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1531,7 +1545,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F25" s="3">
-        <v>0.06</v>
+        <v>6.3965318759402576E-2</v>
       </c>
       <c r="G25" s="4">
         <v>0.91778925619834395</v>
@@ -1543,16 +1557,16 @@
         <v>0.53536660000000003</v>
       </c>
       <c r="J25" s="4">
-        <v>0.14724409448818898</v>
+        <v>0.14565473983355318</v>
       </c>
       <c r="K25" s="4">
-        <v>9.6000000000000002E-2</v>
+        <v>9.5699916455822057E-2</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1569,7 +1583,7 @@
         <v>4.2249999999999996E-2</v>
       </c>
       <c r="F26" s="3">
-        <v>7.22E-2</v>
+        <v>6.7567421147163159E-2</v>
       </c>
       <c r="G26" s="4">
         <v>1.01294685990338</v>
@@ -1581,16 +1595,16 @@
         <v>0.57313510000000001</v>
       </c>
       <c r="J26" s="4">
-        <v>0.13385826771653545</v>
+        <v>0.14417167428263467</v>
       </c>
       <c r="K26" s="4">
-        <v>9.0999999999999998E-2</v>
+        <v>9.0662547572018248E-2</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1607,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="3">
-        <v>5.1900000000000002E-2</v>
+        <v>5.4902949409956894E-2</v>
       </c>
       <c r="G27" s="4">
         <v>1.12787581699346</v>
@@ -1619,13 +1633,13 @@
         <v>0.56558140000000001</v>
       </c>
       <c r="J27" s="4">
-        <v>0.16338582677165356</v>
-      </c>
-      <c r="K27" s="4">
-        <v>0.10154192194819864</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.14995332477297127</v>
+      </c>
+      <c r="K27" s="9">
+        <v>9.8149265780968623E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1642,7 +1656,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="F28" s="3">
-        <v>7.5999999999999998E-2</v>
+        <v>7.5126832560828846E-2</v>
       </c>
       <c r="G28" s="4">
         <v>0.93129411764706205</v>
@@ -1654,13 +1668,13 @@
         <v>0.61090359999999999</v>
       </c>
       <c r="J28" s="4">
-        <v>0.13070866141732285</v>
+        <v>0.14015519678378818</v>
       </c>
       <c r="K28" s="4">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8.1600402447551082E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>6.8499999999999991E-2</v>
       </c>
       <c r="F29" s="3">
-        <v>6.0999999999999999E-2</v>
+        <v>6.6745575323216511E-2</v>
       </c>
       <c r="G29" s="4">
         <v>1.2103846153846101</v>
@@ -1691,7 +1705,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1708,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="3">
-        <v>0.13420000000000001</v>
+        <v>0.12908340299687351</v>
       </c>
       <c r="G30" s="4">
         <v>1.0900000000000001</v>
@@ -1722,7 +1736,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1739,7 +1753,7 @@
         <v>6.6250000000000003E-2</v>
       </c>
       <c r="F31" s="3">
-        <v>0.1007</v>
+        <v>0.1104124870312857</v>
       </c>
       <c r="G31" s="4">
         <v>1.21164062499999</v>
@@ -1751,13 +1765,13 @@
         <v>0.4673833</v>
       </c>
       <c r="J31" s="4">
-        <v>0.15354330708661418</v>
+        <v>0.15890298698925276</v>
       </c>
       <c r="K31" s="4">
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.10791077054099346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1774,7 +1788,7 @@
         <v>5.1249999999999997E-2</v>
       </c>
       <c r="F32" s="3">
-        <v>5.8400000000000001E-2</v>
+        <v>6.2281356621440055E-2</v>
       </c>
       <c r="G32" s="4">
         <v>0.97622641509433805</v>
@@ -1786,13 +1800,13 @@
         <v>0.64867209999999997</v>
       </c>
       <c r="J32" s="4">
-        <v>0.15472440944881891</v>
-      </c>
-      <c r="K32" s="4">
-        <v>0.10101251037412776</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.15882341443647127</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.10113937300653447</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1809,7 +1823,7 @@
         <v>0.04</v>
       </c>
       <c r="F33" s="3">
-        <v>6.0199999999999997E-2</v>
+        <v>6.8015100454286451E-2</v>
       </c>
       <c r="G33" s="4">
         <v>1.1382673267326699</v>
@@ -1821,13 +1835,13 @@
         <v>0.4673833</v>
       </c>
       <c r="J33" s="4">
-        <v>0.15354330708661418</v>
+        <v>0.16322862485600789</v>
       </c>
       <c r="K33" s="4">
-        <v>0.104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.1035468978724587</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1844,7 +1858,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
       <c r="F34" s="3">
-        <v>6.3299999999999995E-2</v>
+        <v>6.5465007664461547E-2</v>
       </c>
       <c r="G34" s="4">
         <v>0.884571428571434</v>
@@ -1856,13 +1870,13 @@
         <v>0.474937</v>
       </c>
       <c r="J34" s="4">
-        <v>0.16023622047244096</v>
+        <v>0.16126747225336144</v>
       </c>
       <c r="K34" s="4">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.8087343362844748E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1879,7 +1893,7 @@
         <v>0.05</v>
       </c>
       <c r="F35" s="3">
-        <v>7.9799999999999996E-2</v>
+        <v>7.5315036103296429E-2</v>
       </c>
       <c r="G35" s="4">
         <v>1.06910869565217</v>
@@ -1891,13 +1905,13 @@
         <v>0.56558140000000001</v>
       </c>
       <c r="J35" s="4">
-        <v>0.11850393700787401</v>
+        <v>0.13016960686688819</v>
       </c>
       <c r="K35" s="4">
-        <v>9.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.2685659508339249E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1914,7 +1928,7 @@
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="F36" s="3">
-        <v>7.0099999999999996E-2</v>
+        <v>6.8095077842878701E-2</v>
       </c>
       <c r="G36" s="4">
         <v>0.93595617529880604</v>
@@ -1926,13 +1940,13 @@
         <v>0.4673833</v>
       </c>
       <c r="J36" s="4">
-        <v>0.14212598425196851</v>
+        <v>0.14814102502561852</v>
       </c>
       <c r="K36" s="4">
-        <v>0.10100000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.10081006593455709</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1949,7 +1963,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F37" s="3">
-        <v>5.3400000000000003E-2</v>
+        <v>5.4674308856766385E-2</v>
       </c>
       <c r="G37" s="4">
         <v>0.87760000000000005</v>
@@ -1961,13 +1975,13 @@
         <v>0.5882425</v>
       </c>
       <c r="J37" s="4">
-        <v>0.13346456692913386</v>
+        <v>0.14634018554959607</v>
       </c>
       <c r="K37" s="4">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.3927402271521993E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1984,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="3">
-        <v>5.8599999999999999E-2</v>
+        <v>5.9875545638368097E-2</v>
       </c>
       <c r="G38" s="4">
         <v>1.1080630630630599</v>
@@ -1996,13 +2010,13 @@
         <v>0.54292030000000002</v>
       </c>
       <c r="J38" s="4">
-        <v>0.1673228346456693</v>
-      </c>
-      <c r="K38" s="4">
-        <v>0.10148699597777602</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.16372974049657166</v>
+      </c>
+      <c r="K38" s="9">
+        <v>0.10279329552139431</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2019,7 +2033,7 @@
         <v>0.06</v>
       </c>
       <c r="F39" s="3">
-        <v>6.8400000000000002E-2</v>
+        <v>7.2914658584322417E-2</v>
       </c>
       <c r="G39" s="4">
         <v>1.07753164556962</v>
@@ -2031,13 +2045,13 @@
         <v>0.4673833</v>
       </c>
       <c r="J39" s="4">
-        <v>0.15905511811023623</v>
+        <v>0.1604674155172193</v>
       </c>
       <c r="K39" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.984611504639386E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2054,7 +2068,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F40" s="3">
-        <v>0.15390000000000001</v>
+        <v>0.13779834771160512</v>
       </c>
       <c r="G40" s="4">
         <v>1.12333333333333</v>
@@ -2068,7 +2082,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2085,7 +2099,7 @@
         <v>0.06</v>
       </c>
       <c r="F41" s="3">
-        <v>6.0999999999999999E-2</v>
+        <v>6.2612796934050349E-2</v>
       </c>
       <c r="G41" s="4">
         <v>0.93315508021390203</v>
@@ -2097,13 +2111,13 @@
         <v>0.474937</v>
       </c>
       <c r="J41" s="4">
-        <v>0.14527559055118111</v>
+        <v>0.15818356162655983</v>
       </c>
       <c r="K41" s="4">
-        <v>0.104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.10407582932119555</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2120,7 +2134,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F42" s="3">
-        <v>7.7700000000000005E-2</v>
+        <v>7.4121446234030289E-2</v>
       </c>
       <c r="G42" s="4">
         <v>0.99818750000000001</v>
@@ -2132,13 +2146,13 @@
         <v>0.55047400000000002</v>
       </c>
       <c r="J42" s="4">
-        <v>0.12165354330708661</v>
+        <v>0.13299346164454842</v>
       </c>
       <c r="K42" s="4">
-        <v>8.3000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8.2714244997922251E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2155,7 +2169,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F43" s="3">
-        <v>5.6800000000000003E-2</v>
+        <v>6.4185045132750848E-2</v>
       </c>
       <c r="G43" s="4">
         <v>0.85303763440860003</v>
@@ -2167,13 +2181,13 @@
         <v>0.4673833</v>
       </c>
       <c r="J43" s="4">
-        <v>0.14409448818897638</v>
+        <v>0.14724762394453977</v>
       </c>
       <c r="K43" s="4">
-        <v>9.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.4974044425572876E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2190,7 +2204,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="F44" s="3">
-        <v>5.3900000000000003E-2</v>
+        <v>5.8844798768475905E-2</v>
       </c>
       <c r="G44" s="4">
         <v>0.90491631799163097</v>
@@ -2202,16 +2216,16 @@
         <v>0.52781290000000003</v>
       </c>
       <c r="J44" s="4">
-        <v>0.14606299212598425</v>
+        <v>0.15315575806623347</v>
       </c>
       <c r="K44" s="4">
-        <v>9.6000000000000002E-2</v>
+        <v>9.5855572553934815E-2</v>
       </c>
       <c r="L44" s="4">
-        <v>2.1495071510795983E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.0017188035609042E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2228,7 +2242,7 @@
         <v>4.8499999999999995E-2</v>
       </c>
       <c r="F45" s="3">
-        <v>5.8999999999999997E-2</v>
+        <v>6.0178981365266664E-2</v>
       </c>
       <c r="G45" s="4">
         <v>1.07424778761061</v>
@@ -2240,13 +2254,13 @@
         <v>0.51270550000000004</v>
       </c>
       <c r="J45" s="4">
-        <v>0.15236220472440945</v>
-      </c>
-      <c r="K45" s="4">
-        <v>0.10071295241200602</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.16513651891400161</v>
+      </c>
+      <c r="K45" s="9">
+        <v>0.10326752052590996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2263,7 +2277,7 @@
         <v>0.06</v>
       </c>
       <c r="F46" s="3">
-        <v>0.1066</v>
+        <v>0.10724131610838705</v>
       </c>
       <c r="G46" s="4">
         <v>1.06</v>
@@ -2277,7 +2291,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2294,7 +2308,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="F47" s="3">
-        <v>6.8599999999999994E-2</v>
+        <v>6.9091991670842123E-2</v>
       </c>
       <c r="G47" s="4">
         <v>0.97886292834890798</v>
@@ -2306,13 +2320,13 @@
         <v>0.48249069999999999</v>
       </c>
       <c r="J47" s="4">
-        <v>0.15748031496062992</v>
-      </c>
-      <c r="K47" s="4">
-        <v>0.10100000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.15688558693483542</v>
+      </c>
+      <c r="K47" s="8">
+        <v>0.1013</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2329,7 +2343,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F48" s="3">
-        <v>4.7100000000000003E-2</v>
+        <v>4.587851939291749E-2</v>
       </c>
       <c r="G48" s="4">
         <v>1.1595070422535101</v>
@@ -2341,13 +2355,11 @@
         <v>0.56558140000000001</v>
       </c>
       <c r="J48" s="4">
-        <v>0.18543307086614175</v>
-      </c>
-      <c r="K48" s="4">
-        <v>9.8855017374080478E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.16367218800720354</v>
+      </c>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2364,7 +2376,7 @@
         <v>0.06</v>
       </c>
       <c r="F49" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>6.4282101258570201E-2</v>
       </c>
       <c r="G49" s="4">
         <v>1.00439999999999</v>
@@ -2376,13 +2388,13 @@
         <v>0.4673833</v>
       </c>
       <c r="J49" s="4">
-        <v>0.15354330708661418</v>
+        <v>0.15473764297466339</v>
       </c>
       <c r="K49" s="4">
-        <v>9.9000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9.9417855198458582E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2399,7 +2411,7 @@
         <v>0.05</v>
       </c>
       <c r="F50" s="3">
-        <v>7.3300000000000004E-2</v>
+        <v>7.6199347018628585E-2</v>
       </c>
       <c r="G50" s="4">
         <v>1.0709574468084999</v>
@@ -2411,13 +2423,13 @@
         <v>0.56558140000000001</v>
       </c>
       <c r="J50" s="4">
-        <v>0.12913385826771653</v>
+        <v>0.1384114536193134</v>
       </c>
       <c r="K50" s="4">
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.10231555818970327</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2434,7 +2446,7 @@
         <v>0.04</v>
       </c>
       <c r="F51" s="3">
-        <v>6.7100000000000007E-2</v>
+        <v>6.6072880235306872E-2</v>
       </c>
       <c r="G51" s="4">
         <v>1.0227906976744101</v>
@@ -2446,174 +2458,183 @@
         <v>0.48249069999999999</v>
       </c>
       <c r="J51" s="4">
-        <v>0.13346456692913386</v>
-      </c>
-      <c r="K51" s="4">
-        <v>9.5922391195530504E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.13878927185101184</v>
+      </c>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F54" s="3"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B80" s="3"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" s="3"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" s="3"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" s="3"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" s="3"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" s="3"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" s="3"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" s="3"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" s="3"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" s="3"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" s="3"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" s="3"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" s="3"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" s="3"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" s="3"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" s="3"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" s="3"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" s="3"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" s="3"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" s="3"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" s="3"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" s="3"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" s="3"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" s="3"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" s="3"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" s="3"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" s="3"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" s="3"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" s="3"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" s="3"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" s="3"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" s="3"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" s="3"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update uncertain parameters and evaluate_IP
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92C5ACE-DE4F-6E4C-9561-D913F4303C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFBD17D-7A1D-5949-8CA3-8E21F09D3D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
@@ -618,9 +618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0865C41F-F8C1-F743-9CC7-E8990FCDD1B0}">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F54" sqref="F54"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
necessary changes to evaluate grain sorghum biorefinery
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Documents/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFCD6C0-8774-CA45-B543-EC759FCDD21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3042B1F1-5E5B-2547-8324-FCF908F95D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>State</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t>CN Price (USD/kg)</t>
+  </si>
+  <si>
+    <t>Incentives Available</t>
+  </si>
+  <si>
+    <t>1,10,18</t>
+  </si>
+  <si>
+    <t>11,12,19</t>
+  </si>
+  <si>
+    <t>3,20</t>
+  </si>
+  <si>
+    <t>14,15</t>
+  </si>
+  <si>
+    <t>Grain Sorghum GWP (kg CO2e/kg)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -305,6 +323,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,8 +641,8 @@
   <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B53" sqref="B53:E103"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,8 +690,12 @@
       <c r="L1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="M1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -709,6 +732,12 @@
       <c r="K2" s="4">
         <v>0.1009798606781888</v>
       </c>
+      <c r="M2" s="11">
+        <v>7</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.26417647245118059</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -740,8 +769,10 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="4">
+        <v>0.22976144522687494</v>
+      </c>
       <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -776,8 +807,10 @@
         <v>0.1828893050111752</v>
       </c>
       <c r="K4" s="4"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="4">
+        <v>0.33279305592023811</v>
+      </c>
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -814,8 +847,10 @@
       <c r="K5" s="4">
         <v>9.9827239610366672E-2</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="4">
+        <v>0.36257689846397995</v>
+      </c>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -852,8 +887,10 @@
       <c r="K6" s="4">
         <v>9.9100060902702611E-2</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="4">
+        <v>0.39373634878453906</v>
+      </c>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -890,8 +927,12 @@
       <c r="K7" s="4">
         <v>0.1005980543403491</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="M7" s="11">
+        <v>8</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.3716013825908942</v>
+      </c>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -924,8 +965,10 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="4">
+        <v>0.23937265809443015</v>
+      </c>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -962,8 +1005,10 @@
       <c r="K9" s="4">
         <v>0.10749740378117047</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="4">
+        <v>0.25958578461867854</v>
+      </c>
       <c r="O9" s="5"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1003,8 +1048,10 @@
       <c r="L10" s="4">
         <v>3.5460462291237851E-2</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="4">
+        <v>0.30389202389290321</v>
+      </c>
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1041,8 +1088,10 @@
       <c r="K11" s="4">
         <v>9.9837507844487458E-2</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="4">
+        <v>0.31046956618637489</v>
+      </c>
       <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1078,8 +1127,12 @@
       <c r="L12" s="9">
         <v>4.1837569088880762E-2</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="M12" s="12">
+        <v>9</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0.39163061512710462</v>
+      </c>
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1114,8 +1167,10 @@
         <v>0.16377798277399688</v>
       </c>
       <c r="K13" s="4"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="4">
+        <v>0.35340612694608214</v>
+      </c>
       <c r="O13" s="5"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1152,8 +1207,10 @@
       <c r="K14" s="4">
         <v>9.9247241347447446E-2</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="4">
+        <v>0.31279858219874584</v>
+      </c>
       <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1190,8 +1247,10 @@
       <c r="K15" s="4">
         <v>9.9621976671312243E-2</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="4">
+        <v>0.21072901053188053</v>
+      </c>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1228,8 +1287,12 @@
       <c r="K16" s="4">
         <v>9.7590485058197077E-2</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="M16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.33375023199982834</v>
+      </c>
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -1266,8 +1329,12 @@
       <c r="K17" s="4">
         <v>9.3021849274127308E-2</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="M17" s="12">
+        <v>2</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0.25997593169021171</v>
+      </c>
       <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1304,8 +1371,12 @@
       <c r="K18" s="4">
         <v>9.4899700034390674E-2</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="M18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0.21726024556862603</v>
+      </c>
       <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1345,8 +1416,12 @@
       <c r="L19" s="4">
         <v>3.0998164400037817E-2</v>
       </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+      <c r="M19" s="12">
+        <v>13</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0.25755971808983813</v>
+      </c>
       <c r="O19" s="5"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1379,8 +1454,10 @@
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="4">
+        <v>0.39372660549121902</v>
+      </c>
       <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -1417,8 +1494,10 @@
       <c r="K21" s="4">
         <v>9.7668460825379097E-2</v>
       </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="4">
+        <v>0.39613486139245963</v>
+      </c>
       <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -1451,8 +1530,10 @@
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="4">
+        <v>0.37204751757560339</v>
+      </c>
       <c r="O22" s="5"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -1489,8 +1570,10 @@
       <c r="K23" s="4">
         <v>0.10254721620128734</v>
       </c>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="4">
+        <v>0.35217405122267709</v>
+      </c>
       <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -1527,8 +1610,10 @@
       <c r="K24" s="4">
         <v>9.6428935997652065E-2</v>
       </c>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="4">
+        <v>0.26321152714905249</v>
+      </c>
       <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -1565,8 +1650,10 @@
       <c r="K25" s="4">
         <v>9.5699916455822057E-2</v>
       </c>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="4">
+        <v>0.39578062740718756</v>
+      </c>
       <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -1603,8 +1690,10 @@
       <c r="K26" s="4">
         <v>9.0662547572018248E-2</v>
       </c>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="4">
+        <v>0.21062110045859775</v>
+      </c>
       <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -1641,6 +1730,12 @@
       <c r="K27" s="9">
         <v>9.8149265780968623E-2</v>
       </c>
+      <c r="M27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0.2439725459438532</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1676,6 +1771,12 @@
       <c r="K28" s="4">
         <v>8.1600402447551082E-2</v>
       </c>
+      <c r="M28" s="11">
+        <v>4</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0.38495382496373831</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1707,6 +1808,10 @@
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="4">
+        <v>0.3440646507665438</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1738,6 +1843,10 @@
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="4">
+        <v>0.37845316974930937</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1773,6 +1882,10 @@
       <c r="K31" s="4">
         <v>0.10791077054099346</v>
       </c>
+      <c r="M31" s="11"/>
+      <c r="N31" s="4">
+        <v>0.39233185644600327</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1808,8 +1921,14 @@
       <c r="K32" s="9">
         <v>0.10113937300653447</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" s="11">
+        <v>6</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0.35777872367086</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1843,8 +1962,12 @@
       <c r="K33" s="4">
         <v>0.1035468978724587</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" s="11"/>
+      <c r="N33" s="4">
+        <v>0.37156941805265903</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1878,8 +2001,12 @@
       <c r="K34" s="4">
         <v>9.8087343362844748E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" s="11"/>
+      <c r="N34" s="4">
+        <v>0.22481436745347783</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1913,8 +2040,12 @@
       <c r="K35" s="4">
         <v>9.2685659508339249E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" s="11"/>
+      <c r="N35" s="4">
+        <v>0.26317000171309046</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1948,8 +2079,12 @@
       <c r="K36" s="4">
         <v>0.10081006593455709</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" s="11"/>
+      <c r="N36" s="4">
+        <v>0.2874424981744802</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1983,8 +2118,12 @@
       <c r="K37" s="4">
         <v>9.3927402271521993E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" s="11"/>
+      <c r="N37" s="4">
+        <v>0.39187528013725292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2018,8 +2157,14 @@
       <c r="K38" s="9">
         <v>0.10279329552139431</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38" s="11">
+        <v>5</v>
+      </c>
+      <c r="N38" s="4">
+        <v>0.20130391386157973</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2053,8 +2198,12 @@
       <c r="K39" s="4">
         <v>9.984611504639386E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" s="11"/>
+      <c r="N39" s="4">
+        <v>0.38157550893993836</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2084,8 +2233,12 @@
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40" s="11"/>
+      <c r="N40" s="4">
+        <v>0.22073469718851083</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2119,8 +2272,14 @@
       <c r="K41" s="4">
         <v>0.10407582932119555</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="N41" s="4">
+        <v>0.20101038122411241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2154,8 +2313,12 @@
       <c r="K42" s="4">
         <v>8.2714244997922251E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" s="11"/>
+      <c r="N42" s="4">
+        <v>0.28345354157893859</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2189,8 +2352,12 @@
       <c r="K43" s="4">
         <v>9.4974044425572876E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" s="11"/>
+      <c r="N43" s="4">
+        <v>0.29715844371645106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2227,8 +2394,12 @@
       <c r="L44" s="4">
         <v>2.0017188035609042E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" s="11"/>
+      <c r="N44" s="4">
+        <v>0.27435700231380244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2262,8 +2433,14 @@
       <c r="K45" s="9">
         <v>0.10326752052590996</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" s="11">
+        <v>16</v>
+      </c>
+      <c r="N45" s="4">
+        <v>0.24662334784600373</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2293,8 +2470,12 @@
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" s="11"/>
+      <c r="N46" s="4">
+        <v>0.34460930459439265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2328,8 +2509,14 @@
       <c r="K47" s="8">
         <v>0.1013</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" s="11">
+        <v>17</v>
+      </c>
+      <c r="N47" s="4">
+        <v>0.38980619309074954</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2361,8 +2548,12 @@
         <v>0.16367218800720354</v>
       </c>
       <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M48" s="11"/>
+      <c r="N48" s="4">
+        <v>0.24822583260737149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2396,8 +2587,12 @@
       <c r="K49" s="4">
         <v>9.9417855198458582E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M49" s="11"/>
+      <c r="N49" s="4">
+        <v>0.38024077437927895</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2431,8 +2626,12 @@
       <c r="K50" s="4">
         <v>0.10231555818970327</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M50" s="11"/>
+      <c r="N50" s="4">
+        <v>0.3614988730813119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2464,13 +2663,17 @@
         <v>0.13878927185101184</v>
       </c>
       <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M51" s="11"/>
+      <c r="N51" s="4">
+        <v>0.38748632964974394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="11"/>
@@ -2484,69 +2687,69 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="11"/>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="11"/>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="11"/>
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="11"/>
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="11"/>

</xml_diff>

<commit_message>
add natural gas prices
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Documents/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFCD6C0-8774-CA45-B543-EC759FCDD21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE7CFA0-295A-8440-8B39-19221AB3A659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>State</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>CN Price (USD/kg)</t>
+  </si>
+  <si>
+    <t>Natural Gas Price (USD/kg)</t>
   </si>
 </sst>
 </file>
@@ -619,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0865C41F-F8C1-F743-9CC7-E8990FCDD1B0}">
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B53" sqref="B53:E103"/>
+      <selection pane="topRight" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,10 +634,11 @@
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,28 +658,31 @@
         <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -694,23 +701,26 @@
       <c r="F2" s="3">
         <v>6.2789131663139625E-2</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2">
+        <v>0.19</v>
+      </c>
+      <c r="H2" s="4">
         <v>0.82354978354978503</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>0.46</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>0.48249069999999999</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>0.15181188116355238</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>0.1009798606781888</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -729,22 +739,25 @@
       <c r="F3" s="3">
         <v>0.16386843710989343</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3">
+        <v>0.26</v>
+      </c>
+      <c r="H3" s="4">
         <v>2.5634722222222202</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="M3" s="5"/>
+      <c r="L3" s="4"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -763,24 +776,27 @@
       <c r="F4" s="3">
         <v>6.6443261853096097E-2</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
+        <v>0.21</v>
+      </c>
+      <c r="H4" s="4">
         <v>0.95596153846153598</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.36</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>0.65622580000000008</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>0.1828893050111752</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="M4" s="5"/>
+      <c r="L4" s="4"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -799,26 +815,29 @@
       <c r="F5" s="3">
         <v>6.1117582891474474E-2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
+        <v>0.34</v>
+      </c>
+      <c r="H5" s="4">
         <v>0.85480952380952302</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.66</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>0.48249069999999999</v>
       </c>
-      <c r="J5" s="8">
+      <c r="K5" s="8">
         <v>0.14752052802935314</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>9.9827239610366672E-2</v>
       </c>
-      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -837,26 +856,29 @@
       <c r="F6" s="3">
         <v>0.12366670610986258</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
+        <v>0.41</v>
+      </c>
+      <c r="H6" s="4">
         <v>1.0981586402266199</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.22</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>0.61090359999999999</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>0.16425594135119409</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>9.9100060902702611E-2</v>
       </c>
-      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -875,26 +897,29 @@
       <c r="F7" s="3">
         <v>7.5577173790691177E-2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
+        <v>0.27</v>
+      </c>
+      <c r="H7" s="4">
         <v>0.99910614525139696</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.36</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>0.63356469999999998</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>0.14313759791125041</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>0.1005980543403491</v>
       </c>
-      <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -913,22 +938,25 @@
       <c r="F8" s="3">
         <v>0.13663525910578617</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8">
+        <v>0.34</v>
+      </c>
+      <c r="H8" s="4">
         <v>1.11506849315068</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.26</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="M8" s="5"/>
+      <c r="L8" s="4"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -947,26 +975,29 @@
       <c r="F9" s="3">
         <v>8.5310311576788742E-2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H9" s="4">
         <v>1.04588235294117</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.47</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>0.16286177082103859</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>0.10749740378117047</v>
       </c>
-      <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -985,29 +1016,32 @@
       <c r="F10" s="3">
         <v>8.2180025132533141E-2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="4">
         <v>0.82572104018912895</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <v>0.5</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>0.474937</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>0.15863061458229014</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>0.10105252773364543</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <v>3.5460462291237851E-2</v>
       </c>
-      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1026,26 +1060,29 @@
       <c r="F11" s="3">
         <v>6.3423978207905019E-2</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11">
+        <v>0.21</v>
+      </c>
+      <c r="H11" s="4">
         <v>0.90413502109704202</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.46</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>0.474937</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>0.16518991256398702</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="4">
         <v>9.9837507844487458E-2</v>
       </c>
-      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1064,25 +1101,28 @@
       <c r="F12" s="3">
         <v>0.26779016263781885</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H12" s="4">
         <v>2.4517088607594899</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>0.9</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="9">
+      <c r="L12" s="4"/>
+      <c r="M12" s="9">
         <v>4.1837569088880762E-2</v>
       </c>
-      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1101,24 +1141,27 @@
       <c r="F13" s="3">
         <v>6.2761533922631604E-2</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="4">
         <v>1.0685826771653499</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.36</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <v>0.55802770000000002</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <v>0.16377798277399688</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="M13" s="5"/>
+      <c r="L13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1137,26 +1180,29 @@
       <c r="F14" s="3">
         <v>6.7262441783450463E-2</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14">
+        <v>0.23</v>
+      </c>
+      <c r="H14" s="4">
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.66</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <v>0.55802770000000002</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>0.14211697862500514</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>9.9247241347447446E-2</v>
       </c>
-      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1175,26 +1221,29 @@
       <c r="F15" s="3">
         <v>7.0590290596535779E-2</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H15" s="4">
         <v>0.921747311827955</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.66</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <v>0.57313510000000001</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>0.14771147761180747</v>
       </c>
-      <c r="K15" s="4">
+      <c r="L15" s="4">
         <v>9.9621976671312243E-2</v>
       </c>
-      <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1213,26 +1262,29 @@
       <c r="F16" s="3">
         <v>6.0891019236762482E-2</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16">
+        <v>0.24</v>
+      </c>
+      <c r="H16" s="4">
         <v>1.05122881355932</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="6">
         <v>0.66</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <v>0.56558140000000001</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <v>0.14093735809892324</v>
       </c>
-      <c r="K16" s="4">
+      <c r="L16" s="4">
         <v>9.7590485058197077E-2</v>
       </c>
-      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1251,26 +1303,29 @@
       <c r="F17" s="3">
         <v>7.5327301796108095E-2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17">
+        <v>0.18</v>
+      </c>
+      <c r="H17" s="4">
         <v>1.02352459016393</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <v>0.67133320000000007</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>0.13986471749870394</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <v>9.3021849274127308E-2</v>
       </c>
-      <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1289,26 +1344,29 @@
       <c r="F18" s="3">
         <v>5.6937146951795831E-2</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18">
+        <v>0.19</v>
+      </c>
+      <c r="H18" s="4">
         <v>0.874117647058822</v>
       </c>
-      <c r="H18" s="7">
+      <c r="I18" s="7">
         <v>0.46499999999999997</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <v>0.49004439999999999</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <v>0.14826754107153112</v>
       </c>
-      <c r="K18" s="4">
+      <c r="L18" s="4">
         <v>9.4899700034390674E-2</v>
       </c>
-      <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1327,29 +1385,32 @@
       <c r="F19" s="3">
         <v>5.6230227333412305E-2</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H19" s="4">
         <v>0.847694805194804</v>
       </c>
-      <c r="H19" s="4">
+      <c r="I19" s="4">
         <v>0.55666666666666675</v>
       </c>
-      <c r="I19" s="4">
+      <c r="J19" s="4">
         <v>0.474937</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <v>0.14599419409541536</v>
       </c>
-      <c r="K19" s="4">
+      <c r="L19" s="4">
         <v>9.904545674243613E-2</v>
       </c>
-      <c r="L19" s="4">
+      <c r="M19" s="4">
         <v>3.0998164400037817E-2</v>
       </c>
-      <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1368,22 +1429,25 @@
       <c r="F20" s="3">
         <v>9.215547040094374E-2</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20">
+        <v>0.42</v>
+      </c>
+      <c r="H20" s="4">
         <v>1.0423026315789401</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>0.26</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="M20" s="5"/>
+      <c r="L20" s="4"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1402,26 +1466,29 @@
       <c r="F21" s="3">
         <v>8.716104866626935E-2</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21">
+        <v>0.48</v>
+      </c>
+      <c r="H21" s="4">
         <v>0.98325966850828705</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>0.47</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J21" s="8">
+      <c r="K21" s="8">
         <v>0.16096259395991458</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="4">
         <v>9.7668460825379097E-2</v>
       </c>
-      <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1440,22 +1507,25 @@
       <c r="F22" s="3">
         <v>0.14155008620047138</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="4">
         <v>1.17718954248365</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>0.26</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <v>0.474937</v>
       </c>
-      <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="M22" s="5"/>
+      <c r="L22" s="4"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1474,26 +1544,29 @@
       <c r="F23" s="3">
         <v>7.5334071429621285E-2</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23">
+        <v>0.32</v>
+      </c>
+      <c r="H23" s="4">
         <v>1.03088372093023</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>0.66</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <v>0.50515179999999993</v>
       </c>
-      <c r="J23" s="8">
+      <c r="K23" s="8">
         <v>0.14361676480793545</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="4">
         <v>0.10254721620128734</v>
       </c>
-      <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1512,26 +1585,29 @@
       <c r="F24" s="3">
         <v>7.28318797422043E-2</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24">
+        <v>0.22</v>
+      </c>
+      <c r="H24" s="4">
         <v>1.0664848484848399</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>0.66</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <v>0.52781290000000003</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <v>0.13573154763419962</v>
       </c>
-      <c r="K24" s="4">
+      <c r="L24" s="4">
         <v>9.6428935997652065E-2</v>
       </c>
-      <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1550,26 +1626,29 @@
       <c r="F25" s="3">
         <v>6.3965318759402576E-2</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25">
+        <v>0.22</v>
+      </c>
+      <c r="H25" s="4">
         <v>0.91778925619834395</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.46</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>0.53536660000000003</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>0.14565473983355318</v>
       </c>
-      <c r="K25" s="4">
+      <c r="L25" s="4">
         <v>9.5699916455822057E-2</v>
       </c>
-      <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1588,26 +1667,29 @@
       <c r="F26" s="3">
         <v>6.7567421147163159E-2</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26">
+        <v>0.31</v>
+      </c>
+      <c r="H26" s="4">
         <v>1.01294685990338</v>
       </c>
-      <c r="H26" s="4">
+      <c r="I26" s="4">
         <v>0.55666666666666675</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <v>0.57313510000000001</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>0.14417167428263467</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>9.0662547572018248E-2</v>
       </c>
-      <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="5"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1626,23 +1708,26 @@
       <c r="F27" s="3">
         <v>5.4902949409956894E-2</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27">
+        <v>0.32</v>
+      </c>
+      <c r="H27" s="4">
         <v>1.12787581699346</v>
       </c>
-      <c r="H27" s="6">
+      <c r="I27" s="6">
         <v>0.36</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <v>0.56558140000000001</v>
       </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
         <v>0.14995332477297127</v>
       </c>
-      <c r="K27" s="9">
+      <c r="L27" s="9">
         <v>9.8149265780968623E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1661,23 +1746,26 @@
       <c r="F28" s="3">
         <v>7.5126832560828846E-2</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28">
+        <v>0.21</v>
+      </c>
+      <c r="H28" s="4">
         <v>0.93129411764706205</v>
       </c>
-      <c r="H28" s="4">
+      <c r="I28" s="4">
         <v>0.60499999999999998</v>
       </c>
-      <c r="I28" s="4">
+      <c r="J28" s="4">
         <v>0.61090359999999999</v>
       </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
         <v>0.14015519678378818</v>
       </c>
-      <c r="K28" s="4">
+      <c r="L28" s="4">
         <v>8.1600402447551082E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1696,19 +1784,22 @@
       <c r="F29" s="3">
         <v>6.6745575323216511E-2</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29">
+        <v>0.32</v>
+      </c>
+      <c r="H29" s="4">
         <v>1.2103846153846101</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>0.36</v>
       </c>
-      <c r="I29" s="4">
+      <c r="J29" s="4">
         <v>0.54292030000000002</v>
       </c>
-      <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1727,19 +1818,22 @@
       <c r="F30" s="3">
         <v>0.12908340299687351</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30">
+        <v>0.46</v>
+      </c>
+      <c r="H30" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>0.26</v>
       </c>
-      <c r="I30" s="4">
+      <c r="J30" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1758,23 +1852,26 @@
       <c r="F31" s="3">
         <v>0.1104124870312857</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31">
+        <v>0.41</v>
+      </c>
+      <c r="H31" s="4">
         <v>1.21164062499999</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>0.47</v>
       </c>
-      <c r="I31" s="4">
+      <c r="J31" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J31" s="4">
+      <c r="K31" s="4">
         <v>0.15890298698925276</v>
       </c>
-      <c r="K31" s="4">
+      <c r="L31" s="4">
         <v>0.10791077054099346</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1793,23 +1890,26 @@
       <c r="F32" s="3">
         <v>6.2281356621440055E-2</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32">
+        <v>0.17</v>
+      </c>
+      <c r="H32" s="4">
         <v>0.97622641509433805</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>0.36</v>
       </c>
-      <c r="I32" s="4">
+      <c r="J32" s="4">
         <v>0.64867209999999997</v>
       </c>
-      <c r="J32" s="4">
+      <c r="K32" s="4">
         <v>0.15882341443647127</v>
       </c>
-      <c r="K32" s="9">
+      <c r="L32" s="9">
         <v>0.10113937300653447</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1828,23 +1928,26 @@
       <c r="F33" s="3">
         <v>6.8015100454286451E-2</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33">
+        <v>0.38</v>
+      </c>
+      <c r="H33" s="4">
         <v>1.1382673267326699</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>0.26</v>
       </c>
-      <c r="I33" s="4">
+      <c r="J33" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J33" s="4">
+      <c r="K33" s="4">
         <v>0.16322862485600789</v>
       </c>
-      <c r="K33" s="4">
+      <c r="L33" s="4">
         <v>0.1035468978724587</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1863,23 +1966,26 @@
       <c r="F34" s="3">
         <v>6.5465007664461547E-2</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H34" s="4">
         <v>0.884571428571434</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>0.46</v>
       </c>
-      <c r="I34" s="4">
+      <c r="J34" s="4">
         <v>0.474937</v>
       </c>
-      <c r="J34" s="4">
+      <c r="K34" s="4">
         <v>0.16126747225336144</v>
       </c>
-      <c r="K34" s="4">
+      <c r="L34" s="4">
         <v>9.8087343362844748E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1898,23 +2004,26 @@
       <c r="F35" s="3">
         <v>7.5315036103296429E-2</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35">
+        <v>0.11</v>
+      </c>
+      <c r="H35" s="4">
         <v>1.06910869565217</v>
       </c>
-      <c r="H35" s="4">
+      <c r="I35" s="4">
         <v>0.60499999999999998</v>
       </c>
-      <c r="I35" s="4">
+      <c r="J35" s="4">
         <v>0.56558140000000001</v>
       </c>
-      <c r="J35" s="4">
+      <c r="K35" s="4">
         <v>0.13016960686688819</v>
       </c>
-      <c r="K35" s="4">
+      <c r="L35" s="4">
         <v>9.2685659508339249E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1933,23 +2042,26 @@
       <c r="F36" s="3">
         <v>6.8095077842878701E-2</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36">
+        <v>0.32</v>
+      </c>
+      <c r="H36" s="4">
         <v>0.93595617529880604</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>0.47</v>
       </c>
-      <c r="I36" s="4">
+      <c r="J36" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J36" s="4">
+      <c r="K36" s="4">
         <v>0.14814102502561852</v>
       </c>
-      <c r="K36" s="4">
+      <c r="L36" s="4">
         <v>0.10081006593455709</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1968,23 +2080,26 @@
       <c r="F37" s="3">
         <v>5.4674308856766385E-2</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37">
+        <v>0.12</v>
+      </c>
+      <c r="H37" s="4">
         <v>0.87760000000000005</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I37" s="4">
+      <c r="J37" s="4">
         <v>0.5882425</v>
       </c>
-      <c r="J37" s="4">
+      <c r="K37" s="4">
         <v>0.14634018554959607</v>
       </c>
-      <c r="K37" s="4">
+      <c r="L37" s="4">
         <v>9.3927402271521993E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2003,23 +2118,26 @@
       <c r="F38" s="3">
         <v>5.9875545638368097E-2</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38">
+        <v>0.26</v>
+      </c>
+      <c r="H38" s="4">
         <v>1.1080630630630599</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>0.36</v>
       </c>
-      <c r="I38" s="4">
+      <c r="J38" s="4">
         <v>0.54292030000000002</v>
       </c>
-      <c r="J38" s="4">
+      <c r="K38" s="4">
         <v>0.16372974049657166</v>
       </c>
-      <c r="K38" s="9">
+      <c r="L38" s="9">
         <v>0.10279329552139431</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2038,23 +2156,26 @@
       <c r="F39" s="3">
         <v>7.2914658584322417E-2</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39">
+        <v>0.43</v>
+      </c>
+      <c r="H39" s="4">
         <v>1.07753164556962</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>0.47</v>
       </c>
-      <c r="I39" s="4">
+      <c r="J39" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J39" s="4">
+      <c r="K39" s="4">
         <v>0.1604674155172193</v>
       </c>
-      <c r="K39" s="4">
+      <c r="L39" s="4">
         <v>9.984611504639386E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2073,19 +2194,22 @@
       <c r="F40" s="3">
         <v>0.13779834771160512</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40">
+        <v>0.49</v>
+      </c>
+      <c r="H40" s="4">
         <v>1.12333333333333</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>0.26</v>
       </c>
-      <c r="I40" s="4">
+      <c r="J40" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2104,23 +2228,26 @@
       <c r="F41" s="3">
         <v>6.2612796934050349E-2</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41">
+        <v>0.21</v>
+      </c>
+      <c r="H41" s="4">
         <v>0.93315508021390203</v>
       </c>
-      <c r="H41" s="6">
+      <c r="I41" s="6">
         <v>0.46</v>
       </c>
-      <c r="I41" s="4">
+      <c r="J41" s="4">
         <v>0.474937</v>
       </c>
-      <c r="J41" s="4">
+      <c r="K41" s="4">
         <v>0.15818356162655983</v>
       </c>
-      <c r="K41" s="4">
+      <c r="L41" s="4">
         <v>0.10407582932119555</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2139,23 +2266,26 @@
       <c r="F42" s="3">
         <v>7.4121446234030289E-2</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42">
+        <v>0.24</v>
+      </c>
+      <c r="H42" s="4">
         <v>0.99818750000000001</v>
       </c>
-      <c r="H42" s="4">
+      <c r="I42" s="4">
         <v>0.60499999999999998</v>
       </c>
-      <c r="I42" s="4">
+      <c r="J42" s="4">
         <v>0.55047400000000002</v>
       </c>
-      <c r="J42" s="4">
+      <c r="K42" s="4">
         <v>0.13299346164454842</v>
       </c>
-      <c r="K42" s="4">
+      <c r="L42" s="4">
         <v>8.2714244997922251E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2174,23 +2304,26 @@
       <c r="F43" s="3">
         <v>6.4185045132750848E-2</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43">
+        <v>0.22</v>
+      </c>
+      <c r="H43" s="4">
         <v>0.85303763440860003</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>0.46</v>
       </c>
-      <c r="I43" s="4">
+      <c r="J43" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J43" s="4">
+      <c r="K43" s="4">
         <v>0.14724762394453977</v>
       </c>
-      <c r="K43" s="4">
+      <c r="L43" s="4">
         <v>9.4974044425572876E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2209,26 +2342,29 @@
       <c r="F44" s="3">
         <v>5.8844798768475905E-2</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44">
+        <v>0.12</v>
+      </c>
+      <c r="H44" s="4">
         <v>0.90491631799163097</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>0.47</v>
       </c>
-      <c r="I44" s="4">
+      <c r="J44" s="4">
         <v>0.52781290000000003</v>
       </c>
-      <c r="J44" s="4">
+      <c r="K44" s="4">
         <v>0.15315575806623347</v>
       </c>
-      <c r="K44" s="4">
+      <c r="L44" s="4">
         <v>9.5855572553934815E-2</v>
       </c>
-      <c r="L44" s="4">
+      <c r="M44" s="4">
         <v>2.0017188035609042E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2247,23 +2383,26 @@
       <c r="F45" s="3">
         <v>6.0178981365266664E-2</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45">
+        <v>0.27</v>
+      </c>
+      <c r="H45" s="4">
         <v>1.07424778761061</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>0.36</v>
       </c>
-      <c r="I45" s="4">
+      <c r="J45" s="4">
         <v>0.51270550000000004</v>
       </c>
-      <c r="J45" s="4">
+      <c r="K45" s="4">
         <v>0.16513651891400161</v>
       </c>
-      <c r="K45" s="9">
+      <c r="L45" s="9">
         <v>0.10326752052590996</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2282,19 +2421,22 @@
       <c r="F46" s="3">
         <v>0.10724131610838705</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46">
+        <v>0.19</v>
+      </c>
+      <c r="H46" s="4">
         <v>1.06</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>0.26</v>
       </c>
-      <c r="I46" s="4">
+      <c r="J46" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2313,23 +2455,26 @@
       <c r="F47" s="3">
         <v>6.9091991670842123E-2</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47">
+        <v>0.2</v>
+      </c>
+      <c r="H47" s="4">
         <v>0.97886292834890798</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>0.47</v>
       </c>
-      <c r="I47" s="4">
+      <c r="J47" s="4">
         <v>0.48249069999999999</v>
       </c>
-      <c r="J47" s="4">
+      <c r="K47" s="4">
         <v>0.15688558693483542</v>
       </c>
-      <c r="K47" s="8">
+      <c r="L47" s="8">
         <v>0.1013</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2348,21 +2493,24 @@
       <c r="F48" s="3">
         <v>4.587851939291749E-2</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48">
+        <v>0.42</v>
+      </c>
+      <c r="H48" s="4">
         <v>1.1595070422535101</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>0.36</v>
       </c>
-      <c r="I48" s="4">
+      <c r="J48" s="4">
         <v>0.56558140000000001</v>
       </c>
-      <c r="J48" s="4">
+      <c r="K48" s="4">
         <v>0.16367218800720354</v>
       </c>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2381,23 +2529,26 @@
       <c r="F49" s="3">
         <v>6.4282101258570201E-2</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49">
+        <v>0.13</v>
+      </c>
+      <c r="H49" s="4">
         <v>1.00439999999999</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>0.47</v>
       </c>
-      <c r="I49" s="4">
+      <c r="J49" s="4">
         <v>0.4673833</v>
       </c>
-      <c r="J49" s="4">
+      <c r="K49" s="4">
         <v>0.15473764297466339</v>
       </c>
-      <c r="K49" s="4">
+      <c r="L49" s="4">
         <v>9.9417855198458582E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2416,23 +2567,26 @@
       <c r="F50" s="3">
         <v>7.6199347018628585E-2</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50">
+        <v>0.24</v>
+      </c>
+      <c r="H50" s="4">
         <v>1.0709574468084999</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>0.66</v>
       </c>
-      <c r="I50" s="4">
+      <c r="J50" s="4">
         <v>0.56558140000000001</v>
       </c>
-      <c r="J50" s="4">
+      <c r="K50" s="4">
         <v>0.1384114536193134</v>
       </c>
-      <c r="K50" s="4">
+      <c r="L50" s="4">
         <v>0.10231555818970327</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2451,102 +2605,105 @@
       <c r="F51" s="3">
         <v>6.6072880235306872E-2</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51">
+        <v>0.22</v>
+      </c>
+      <c r="H51" s="4">
         <v>1.0227906976744101</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>0.36</v>
       </c>
-      <c r="I51" s="4">
+      <c r="J51" s="4">
         <v>0.48249069999999999</v>
       </c>
-      <c r="J51" s="4">
+      <c r="K51" s="4">
         <v>0.13878927185101184</v>
       </c>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="11"/>
       <c r="E53" s="10"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53" s="3"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="11"/>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="11"/>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="11"/>
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="11"/>
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="11"/>
@@ -2854,8 +3011,8 @@
       <c r="B119" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:O26">
-    <sortCondition ref="O3:O26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:P26">
+    <sortCondition ref="P3:P26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update state-specific data file
</commit_message>
<xml_diff>
--- a/blocs/incentives/state_scenarios_for_import.xlsx
+++ b/blocs/incentives/state_scenarios_for_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Documents/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744B07E9-5344-694A-BF3B-A1CEC9E13953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB471A38-9CDA-3244-9629-D5EED4AB7A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19520" xr2:uid="{163DA801-9318-4945-BD14-C5631C7A2B18}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>State</t>
   </si>
@@ -223,6 +223,39 @@
   </si>
   <si>
     <t>Natural Gas Price (USD/kg)</t>
+  </si>
+  <si>
+    <t>SD Corn Distance [km]</t>
+  </si>
+  <si>
+    <t>SD Corn Stover Distance [km]</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>Manitoba</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Saskatchewan</t>
+  </si>
+  <si>
+    <t>Quebec</t>
+  </si>
+  <si>
+    <t>LCFS Distance [km]</t>
+  </si>
+  <si>
+    <t>RFS Distance [km]</t>
+  </si>
+  <si>
+    <t>CFR Distance [km]</t>
+  </si>
+  <si>
+    <t>MISC GWP [kg CO2-eq/kg]</t>
   </si>
 </sst>
 </file>
@@ -290,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -307,6 +340,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,11 +655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0865C41F-F8C1-F743-9CC7-E8990FCDD1B0}">
-  <dimension ref="A1:P119"/>
+  <dimension ref="A1:U119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,7 +671,7 @@
     <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,11 +711,26 @@
       <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -718,8 +767,12 @@
       <c r="L2" s="4">
         <v>0.1009798606781888</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S2" s="4">
+        <v>-9.4085339738322171E-2</v>
+      </c>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -755,8 +808,10 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="5"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -791,11 +846,23 @@
         <v>0.1828893050111752</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="N4" s="5"/>
+      <c r="N4" s="11">
+        <v>1500</v>
+      </c>
       <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P4" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>900</v>
+      </c>
+      <c r="R4" s="5">
+        <v>2000</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="11"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -832,11 +899,16 @@
       <c r="L5" s="4">
         <v>9.9827239610366672E-2</v>
       </c>
-      <c r="N5" s="5"/>
+      <c r="N5" s="12"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="5"/>
+      <c r="S5" s="4">
+        <v>-0.17374971421375321</v>
+      </c>
+      <c r="T5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -873,11 +945,25 @@
       <c r="L6" s="4">
         <v>9.9100060902702611E-2</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N6" s="11">
+        <v>1900</v>
+      </c>
+      <c r="O6" s="11">
+        <v>1900</v>
+      </c>
+      <c r="P6" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>200</v>
+      </c>
+      <c r="R6" s="5">
+        <v>1700</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="11"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -914,11 +1000,23 @@
       <c r="L7" s="4">
         <v>0.1005980543403491</v>
       </c>
-      <c r="N7" s="5"/>
+      <c r="N7" s="11">
+        <v>800</v>
+      </c>
       <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P7" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>1300</v>
+      </c>
+      <c r="R7" s="5">
+        <v>1500</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -951,11 +1049,16 @@
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="N8" s="5"/>
+      <c r="N8" s="12"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="5"/>
+      <c r="S8" s="4">
+        <v>-6.8803285354366264E-2</v>
+      </c>
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -992,11 +1095,16 @@
       <c r="L9" s="4">
         <v>0.10749740378117047</v>
       </c>
-      <c r="N9" s="5"/>
+      <c r="N9" s="12"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="5"/>
+      <c r="S9" s="4">
+        <v>-7.2924611112051618E-2</v>
+      </c>
+      <c r="T9" s="11"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1036,11 +1144,16 @@
       <c r="M10" s="4">
         <v>3.5460462291237851E-2</v>
       </c>
-      <c r="N10" s="5"/>
+      <c r="N10" s="12"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="5"/>
+      <c r="S10" s="4">
+        <v>-4.0801288463293742E-2</v>
+      </c>
+      <c r="T10" s="11"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1077,11 +1190,16 @@
       <c r="L11" s="4">
         <v>9.9837507844487458E-2</v>
       </c>
-      <c r="N11" s="5"/>
+      <c r="N11" s="12"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="5"/>
+      <c r="S11" s="4">
+        <v>-5.6783343140775183E-2</v>
+      </c>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1117,11 +1235,14 @@
       <c r="M12" s="9">
         <v>4.1837569088880762E-2</v>
       </c>
-      <c r="N12" s="5"/>
+      <c r="N12" s="12"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" s="5"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="11"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1156,11 +1277,23 @@
         <v>0.16377798277399688</v>
       </c>
       <c r="L13" s="4"/>
-      <c r="N13" s="5"/>
+      <c r="N13" s="11">
+        <v>1200</v>
+      </c>
       <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P13" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>900</v>
+      </c>
+      <c r="R13" s="5">
+        <v>1000</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="11"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1197,11 +1330,25 @@
       <c r="L14" s="4">
         <v>9.9247241347447446E-2</v>
       </c>
-      <c r="N14" s="5"/>
+      <c r="N14" s="11">
+        <v>1100</v>
+      </c>
       <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P14" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>2700</v>
+      </c>
+      <c r="R14" s="5">
+        <v>1100</v>
+      </c>
+      <c r="S14" s="4">
+        <v>-0.17593877386800144</v>
+      </c>
+      <c r="T14" s="11"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1238,11 +1385,25 @@
       <c r="L15" s="4">
         <v>9.9621976671312243E-2</v>
       </c>
-      <c r="N15" s="5"/>
+      <c r="N15" s="11">
+        <v>1300</v>
+      </c>
       <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P15" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>3000</v>
+      </c>
+      <c r="R15" s="5">
+        <v>900</v>
+      </c>
+      <c r="S15" s="4">
+        <v>-0.15298844793452085</v>
+      </c>
+      <c r="T15" s="11"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1279,11 +1440,27 @@
       <c r="L16" s="4">
         <v>9.7590485058197077E-2</v>
       </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N16" s="11">
+        <v>700</v>
+      </c>
+      <c r="O16" s="11">
+        <v>700</v>
+      </c>
+      <c r="P16" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>2400</v>
+      </c>
+      <c r="R16" s="5">
+        <v>1200</v>
+      </c>
+      <c r="S16" s="4">
+        <v>-0.16391720762040199</v>
+      </c>
+      <c r="T16" s="11"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1320,11 +1497,27 @@
       <c r="L17" s="4">
         <v>9.3021849274127308E-2</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N17" s="11">
+        <v>700</v>
+      </c>
+      <c r="O17" s="11">
+        <v>700</v>
+      </c>
+      <c r="P17" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>1900</v>
+      </c>
+      <c r="R17" s="5">
+        <v>1500</v>
+      </c>
+      <c r="S17" s="4">
+        <v>-0.11575785283585475</v>
+      </c>
+      <c r="T17" s="11"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1361,11 +1554,25 @@
       <c r="L18" s="4">
         <v>9.4899700034390674E-2</v>
       </c>
-      <c r="N18" s="5"/>
+      <c r="N18" s="11">
+        <v>1500</v>
+      </c>
       <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P18" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>3100</v>
+      </c>
+      <c r="R18" s="5">
+        <v>1000</v>
+      </c>
+      <c r="S18" s="4">
+        <v>-0.10601355927630496</v>
+      </c>
+      <c r="T18" s="11"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1405,11 +1612,16 @@
       <c r="M19" s="4">
         <v>3.0998164400037817E-2</v>
       </c>
-      <c r="N19" s="5"/>
+      <c r="N19" s="12"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19" s="5"/>
+      <c r="S19" s="4">
+        <v>-8.1968360647978245E-2</v>
+      </c>
+      <c r="T19" s="11"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1442,11 +1654,16 @@
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="N20" s="5"/>
+      <c r="N20" s="12"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20" s="5"/>
+      <c r="S20" s="4">
+        <v>-7.112607060916093E-2</v>
+      </c>
+      <c r="T20" s="11"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1483,11 +1700,16 @@
       <c r="L21" s="4">
         <v>9.7668460825379097E-2</v>
       </c>
-      <c r="N21" s="5"/>
+      <c r="N21" s="12"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q21" s="5"/>
+      <c r="S21" s="4">
+        <v>-9.6688325863235502E-2</v>
+      </c>
+      <c r="T21" s="11"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1520,11 +1742,16 @@
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="5"/>
+      <c r="N22" s="12"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22" s="5"/>
+      <c r="S22" s="4">
+        <v>-7.4083269151241665E-2</v>
+      </c>
+      <c r="T22" s="11"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1561,11 +1788,25 @@
       <c r="L23" s="4">
         <v>0.10254721620128734</v>
       </c>
-      <c r="N23" s="5"/>
+      <c r="N23" s="12">
+        <v>1300</v>
+      </c>
       <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P23" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>3100</v>
+      </c>
+      <c r="R23" s="5">
+        <v>600</v>
+      </c>
+      <c r="S23" s="4">
+        <v>-0.15110066411628251</v>
+      </c>
+      <c r="T23" s="11"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1602,11 +1843,25 @@
       <c r="L24" s="4">
         <v>9.6428935997652065E-2</v>
       </c>
-      <c r="N24" s="5"/>
+      <c r="N24" s="11">
+        <v>500</v>
+      </c>
       <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P24" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>2400</v>
+      </c>
+      <c r="R24" s="5">
+        <v>700</v>
+      </c>
+      <c r="S24" s="4">
+        <v>-0.16100069275580803</v>
+      </c>
+      <c r="T24" s="11"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1643,11 +1898,16 @@
       <c r="L25" s="4">
         <v>9.5699916455822057E-2</v>
       </c>
-      <c r="N25" s="5"/>
+      <c r="N25" s="12"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q25" s="5"/>
+      <c r="S25" s="4">
+        <v>-0.12654163560917234</v>
+      </c>
+      <c r="T25" s="11"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1684,11 +1944,25 @@
       <c r="L26" s="4">
         <v>9.0662547572018248E-2</v>
       </c>
-      <c r="N26" s="5"/>
+      <c r="N26" s="11">
+        <v>1000</v>
+      </c>
       <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P26" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>2500</v>
+      </c>
+      <c r="R26" s="5">
+        <v>1500</v>
+      </c>
+      <c r="S26" s="4">
+        <v>-0.13027280643054095</v>
+      </c>
+      <c r="T26" s="11"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1725,8 +1999,11 @@
       <c r="L27" s="9">
         <v>9.8149265780968623E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N27" s="11"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="11"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1763,8 +2040,24 @@
       <c r="L28" s="4">
         <v>8.1600402447551082E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N28" s="11">
+        <v>400</v>
+      </c>
+      <c r="P28" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q28">
+        <v>1900</v>
+      </c>
+      <c r="R28">
+        <v>1200</v>
+      </c>
+      <c r="S28" s="4">
+        <v>-0.21094360898411893</v>
+      </c>
+      <c r="T28" s="11"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1797,8 +2090,11 @@
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N29" s="11"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="11"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1831,8 +2127,13 @@
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N30" s="11"/>
+      <c r="S30" s="4">
+        <v>-6.8809682789543469E-2</v>
+      </c>
+      <c r="T30" s="11"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1869,8 +2170,13 @@
       <c r="L31" s="4">
         <v>0.10791077054099346</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N31" s="11"/>
+      <c r="S31" s="4">
+        <v>-6.9910530993911826E-2</v>
+      </c>
+      <c r="T31" s="11"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1907,8 +2213,11 @@
       <c r="L32" s="9">
         <v>0.10113937300653447</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" s="11"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="11"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1945,8 +2254,24 @@
       <c r="L33" s="4">
         <v>0.1035468978724587</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="11">
+        <v>2000</v>
+      </c>
+      <c r="P33" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q33">
+        <v>3800</v>
+      </c>
+      <c r="R33">
+        <v>300</v>
+      </c>
+      <c r="S33" s="4">
+        <v>-7.982162411863758E-2</v>
+      </c>
+      <c r="T33" s="11"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1983,8 +2308,24 @@
       <c r="L34" s="4">
         <v>9.8087343362844748E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="11">
+        <v>2100</v>
+      </c>
+      <c r="P34" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q34">
+        <v>3700</v>
+      </c>
+      <c r="R34">
+        <v>1100</v>
+      </c>
+      <c r="S34" s="4">
+        <v>-7.5915493366728828E-2</v>
+      </c>
+      <c r="T34" s="11"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2021,8 +2362,24 @@
       <c r="L35" s="4">
         <v>9.2685659508339249E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="11">
+        <v>400</v>
+      </c>
+      <c r="P35" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q35">
+        <v>2000</v>
+      </c>
+      <c r="R35">
+        <v>700</v>
+      </c>
+      <c r="S35" s="4">
+        <v>-0.18399505103459782</v>
+      </c>
+      <c r="T35" s="11"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2059,8 +2416,24 @@
       <c r="L36" s="4">
         <v>0.10081006593455709</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="11">
+        <v>1600</v>
+      </c>
+      <c r="P36" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q36">
+        <v>3300</v>
+      </c>
+      <c r="R36">
+        <v>700</v>
+      </c>
+      <c r="S36" s="4">
+        <v>-0.164112847688446</v>
+      </c>
+      <c r="T36" s="11"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2097,8 +2470,13 @@
       <c r="L37" s="4">
         <v>9.3927402271521993E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="11"/>
+      <c r="S37" s="4">
+        <v>-0.12881746519999937</v>
+      </c>
+      <c r="T37" s="11"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2135,8 +2513,22 @@
       <c r="L38" s="9">
         <v>0.10279329552139431</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" s="11">
+        <v>1700</v>
+      </c>
+      <c r="P38" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q38">
+        <v>800</v>
+      </c>
+      <c r="R38">
+        <v>1000</v>
+      </c>
+      <c r="S38" s="4"/>
+      <c r="T38" s="11"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2173,8 +2565,24 @@
       <c r="L39" s="4">
         <v>9.984611504639386E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" s="11">
+        <v>1900</v>
+      </c>
+      <c r="P39" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q39">
+        <v>3700</v>
+      </c>
+      <c r="R39">
+        <v>500</v>
+      </c>
+      <c r="S39" s="4">
+        <v>-0.20356695937285976</v>
+      </c>
+      <c r="T39" s="11"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2207,8 +2615,11 @@
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" s="11"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="11"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2245,8 +2656,13 @@
       <c r="L41" s="4">
         <v>0.10407582932119555</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" s="11"/>
+      <c r="S41" s="4">
+        <v>-6.5530580984162021E-2</v>
+      </c>
+      <c r="T41" s="11"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2283,8 +2699,24 @@
       <c r="L42" s="4">
         <v>8.2714244997922251E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" s="11">
+        <v>100</v>
+      </c>
+      <c r="P42" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q42">
+        <v>1900</v>
+      </c>
+      <c r="R42">
+        <v>900</v>
+      </c>
+      <c r="S42" s="4">
+        <v>-0.24543176448711423</v>
+      </c>
+      <c r="T42" s="11"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2321,8 +2753,24 @@
       <c r="L43" s="4">
         <v>9.4974044425572876E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" s="11">
+        <v>1600</v>
+      </c>
+      <c r="P43" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q43">
+        <v>3000</v>
+      </c>
+      <c r="R43">
+        <v>1300</v>
+      </c>
+      <c r="S43" s="4">
+        <v>-0.11931241924960508</v>
+      </c>
+      <c r="T43" s="11"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2362,8 +2810,24 @@
       <c r="M44" s="4">
         <v>2.0017188035609042E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" s="11">
+        <v>1500</v>
+      </c>
+      <c r="P44" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q44" s="11">
+        <v>2000</v>
+      </c>
+      <c r="R44">
+        <v>2400</v>
+      </c>
+      <c r="S44" s="4">
+        <v>-0.14402888674080458</v>
+      </c>
+      <c r="T44" s="11"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2400,8 +2864,11 @@
       <c r="L45" s="9">
         <v>0.10326752052590996</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" s="11"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="11"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2434,8 +2901,13 @@
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46" s="11"/>
+      <c r="S46" s="4">
+        <v>-5.6849278564189934E-2</v>
+      </c>
+      <c r="T46" s="11"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2472,8 +2944,13 @@
       <c r="L47" s="8">
         <v>0.1013</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" s="11"/>
+      <c r="S47" s="4">
+        <v>-9.0021657212510695E-2</v>
+      </c>
+      <c r="T47" s="11"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2508,8 +2985,11 @@
         <v>0.16367218800720354</v>
       </c>
       <c r="L48" s="4"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N48" s="11"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="11"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2546,8 +3026,13 @@
       <c r="L49" s="4">
         <v>9.9417855198458582E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N49" s="11"/>
+      <c r="S49" s="4">
+        <v>-9.2354905056813236E-2</v>
+      </c>
+      <c r="T49" s="11"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2584,8 +3069,27 @@
       <c r="L50" s="4">
         <v>0.10231555818970327</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N50" s="11">
+        <v>900</v>
+      </c>
+      <c r="O50" s="11">
+        <v>900</v>
+      </c>
+      <c r="P50" s="5">
+        <v>200</v>
+      </c>
+      <c r="Q50">
+        <v>2700</v>
+      </c>
+      <c r="R50">
+        <v>700</v>
+      </c>
+      <c r="S50" s="4">
+        <v>-0.10947710424959588</v>
+      </c>
+      <c r="T50" s="11"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2620,13 +3124,19 @@
         <v>0.13878927185101184</v>
       </c>
       <c r="L51" s="4"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S51" s="4"/>
+      <c r="T51" s="11"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="T52" s="11"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="11"/>
@@ -2638,71 +3148,153 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N53" s="11">
+        <v>1300</v>
+      </c>
+      <c r="P53">
+        <v>700</v>
+      </c>
+      <c r="Q53">
+        <v>1800</v>
+      </c>
+      <c r="R53">
+        <v>200</v>
+      </c>
+      <c r="T53" s="11"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
       <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N54">
+        <v>900</v>
+      </c>
+      <c r="P54">
+        <v>700</v>
+      </c>
+      <c r="Q54">
+        <v>2400</v>
+      </c>
+      <c r="R54">
+        <v>200</v>
+      </c>
+      <c r="T54" s="11"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="11"/>
       <c r="E55" s="10"/>
       <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N55">
+        <v>1800</v>
+      </c>
+      <c r="O55">
+        <v>1800</v>
+      </c>
+      <c r="P55">
+        <v>300</v>
+      </c>
+      <c r="Q55">
+        <v>3600</v>
+      </c>
+      <c r="R55">
+        <v>200</v>
+      </c>
+      <c r="T55" s="11"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="11"/>
       <c r="E56" s="10"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N56">
+        <v>900</v>
+      </c>
+      <c r="P56">
+        <v>700</v>
+      </c>
+      <c r="Q56">
+        <v>2000</v>
+      </c>
+      <c r="R56">
+        <v>200</v>
+      </c>
+      <c r="T56" s="11"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="11"/>
       <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N57">
+        <v>2100</v>
+      </c>
+      <c r="O57">
+        <v>2100</v>
+      </c>
+      <c r="P57">
+        <v>300</v>
+      </c>
+      <c r="Q57">
+        <v>3900</v>
+      </c>
+      <c r="R57">
+        <v>200</v>
+      </c>
+      <c r="T57" s="11"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="11"/>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="11"/>
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="11"/>
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="11"/>
@@ -3010,8 +3602,8 @@
       <c r="B119" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:P26">
-    <sortCondition ref="P3:P26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:Q26">
+    <sortCondition ref="Q3:Q26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>